<commit_message>
updating NN results file
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sensata2com-my.sharepoint.com/personal/sofithcheallaigh_sensata_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4813ABE4-339A-413F-8220-E41DC710BFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667DE4F5-5099-43B1-99B6-BD71596FAED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Keras Seq" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="Keras Seq" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="25">
   <si>
     <t xml:space="preserve">Model: </t>
   </si>
@@ -108,6 +109,9 @@
   <si>
     <t>Acc</t>
   </si>
+  <si>
+    <t>2,10</t>
+  </si>
 </sst>
 </file>
 
@@ -459,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,7 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -521,61 +525,73 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -596,6 +612,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>258147</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>86513</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C4817F-C5D0-351D-D601-B75D5BC6BB50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8534400" y="190500"/>
+          <a:ext cx="6963747" cy="5649113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -644,7 +709,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1033,20 +1098,696 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9512EAE-7E03-4C9A-9560-62E0DE7C04A5}">
+  <dimension ref="A2:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="40"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
+        <v>2</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="26">
+        <v>10</v>
+      </c>
+      <c r="H7" s="26">
+        <v>16</v>
+      </c>
+      <c r="I7" s="26">
+        <v>2.4950000000000001</v>
+      </c>
+      <c r="J7" s="42">
+        <v>8.2260000000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>2</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="41">
+        <v>10</v>
+      </c>
+      <c r="H8" s="41">
+        <v>32</v>
+      </c>
+      <c r="I8" s="41">
+        <v>2.4569999999999999</v>
+      </c>
+      <c r="J8" s="43">
+        <v>8.1890000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>2</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="41">
+        <v>10</v>
+      </c>
+      <c r="H9" s="41">
+        <v>64</v>
+      </c>
+      <c r="I9" s="41">
+        <v>2.4630000000000001</v>
+      </c>
+      <c r="J9" s="43">
+        <v>8.1940000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>2</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="41">
+        <v>10</v>
+      </c>
+      <c r="H10" s="41">
+        <v>128</v>
+      </c>
+      <c r="I10" s="41">
+        <v>2.129</v>
+      </c>
+      <c r="J10" s="43">
+        <v>6.2149999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>2</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="41">
+        <v>10</v>
+      </c>
+      <c r="H11" s="41">
+        <v>256</v>
+      </c>
+      <c r="I11" s="41">
+        <v>2.4710000000000001</v>
+      </c>
+      <c r="J11" s="43">
+        <v>8.2080000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>2</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="41">
+        <v>10</v>
+      </c>
+      <c r="H12" s="41">
+        <v>512</v>
+      </c>
+      <c r="I12" s="41">
+        <v>2.4649999999999999</v>
+      </c>
+      <c r="J12" s="24">
+        <v>8.1989999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>2</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="41">
+        <v>10</v>
+      </c>
+      <c r="H13" s="41">
+        <v>1028</v>
+      </c>
+      <c r="I13" s="41">
+        <v>2.4729999999999999</v>
+      </c>
+      <c r="J13" s="24">
+        <v>8.2110000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>2</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6">
+        <v>10</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2056</v>
+      </c>
+      <c r="I14" s="6">
+        <v>2.4620000000000002</v>
+      </c>
+      <c r="J14" s="7">
+        <v>8.2059999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
+        <v>2</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="26">
+        <v>20</v>
+      </c>
+      <c r="H15" s="26">
+        <v>16</v>
+      </c>
+      <c r="I15" s="26">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="J15" s="42">
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="41">
+        <v>2</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="23">
+        <v>20</v>
+      </c>
+      <c r="H16" s="41">
+        <v>32</v>
+      </c>
+      <c r="I16" s="41">
+        <v>2.456</v>
+      </c>
+      <c r="J16" s="41">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="41">
+        <v>2</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="23">
+        <v>20</v>
+      </c>
+      <c r="H17" s="41">
+        <v>64</v>
+      </c>
+      <c r="I17" s="41">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="J17" s="41">
+        <v>5.2779999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="41">
+        <v>2</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="23">
+        <v>20</v>
+      </c>
+      <c r="H18" s="41">
+        <v>128</v>
+      </c>
+      <c r="I18" s="41">
+        <v>2.4580000000000002</v>
+      </c>
+      <c r="J18" s="41">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="41">
+        <v>2</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="23">
+        <v>20</v>
+      </c>
+      <c r="H19" s="41">
+        <v>256</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2.4460000000000002</v>
+      </c>
+      <c r="J19" s="1">
+        <v>8.2010000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:J5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCBFCE0-D62A-4787-8AAA-20AB7ACA5ECA}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
+    <col min="3" max="10" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1054,7 +1795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,123 +1803,123 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="40"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
-        <v>2</v>
-      </c>
-      <c r="B6" s="28" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
+        <v>2</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="28">
+      <c r="C6" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="26">
         <v>10</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="26">
         <v>16</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="26">
         <v>2.4470000000000001</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="27">
         <v>8.1850000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="22">
-        <v>2</v>
-      </c>
-      <c r="B7" s="23" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="23">
+      <c r="C7" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1">
         <v>10</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="1">
         <v>32</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="1">
         <v>0.45</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="24">
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="31">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
         <v>2</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -1205,12 +1946,12 @@
       <c r="I8" s="13">
         <v>0.65600000000000003</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="29">
         <v>0.877</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="33">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
         <v>2</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -1237,44 +1978,44 @@
       <c r="I9" s="19">
         <v>0.61399999999999999</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="31">
         <v>0.85399999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
-        <v>2</v>
-      </c>
-      <c r="B10" s="23" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="23">
+      <c r="C10" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1">
         <v>10</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="1">
         <v>128</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="1">
         <v>0.72299999999999998</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="24">
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="31">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="28">
         <v>2</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -1301,12 +2042,12 @@
       <c r="I11" s="13">
         <v>0.45400000000000001</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="29">
         <v>0.34599999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="32">
         <v>2</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -1333,12 +2074,12 @@
       <c r="I12" s="16">
         <v>0.67900000000000005</v>
       </c>
-      <c r="J12" s="36">
+      <c r="J12" s="33">
         <v>0.83299999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
         <v>2</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -1365,12 +2106,12 @@
       <c r="I13" s="16">
         <v>0.72</v>
       </c>
-      <c r="J13" s="36">
+      <c r="J13" s="33">
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="33">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
         <v>2</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -1397,12 +2138,12 @@
       <c r="I14" s="19">
         <v>0.443</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="31">
         <v>0.311</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="31">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="28">
         <v>2</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -1429,12 +2170,12 @@
       <c r="I15" s="13">
         <v>2.464</v>
       </c>
-      <c r="J15" s="32">
+      <c r="J15" s="29">
         <v>8.202</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="33">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="30">
         <v>2</v>
       </c>
       <c r="B16" s="19" t="s">
@@ -1461,43 +2202,43 @@
       <c r="I16" s="19">
         <v>2.4649999999999999</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="31">
         <v>8.1869999999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="22">
-        <v>2</v>
-      </c>
-      <c r="B17" s="23" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="23">
+      <c r="C17" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="1">
         <v>10</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="1">
         <v>1024</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="1">
         <v>2.4620000000000002</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="24">
         <v>8.1929999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>2</v>
       </c>
@@ -1519,7 +2260,7 @@
       <c r="G18" s="6">
         <v>10</v>
       </c>
-      <c r="H18" s="37">
+      <c r="H18" s="6">
         <v>4096</v>
       </c>
       <c r="I18" s="6">
@@ -1529,23 +2270,23 @@
         <v>8190</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="23">
-        <v>2</v>
-      </c>
-      <c r="B19" s="23" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="24" t="s">
+      <c r="C19" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="22" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="1">
@@ -1561,23 +2302,23 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
-        <v>2</v>
-      </c>
-      <c r="B20" s="23" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="24" t="s">
+      <c r="C20" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="22" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="1">
@@ -1593,23 +2334,23 @@
         <v>0.90500000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="23">
-        <v>2</v>
-      </c>
-      <c r="B21" s="23" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="24" t="s">
+      <c r="C21" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="22" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="1">
@@ -1625,23 +2366,23 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="23">
-        <v>2</v>
-      </c>
-      <c r="B22" s="23" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="24" t="s">
+      <c r="C22" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="22" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="1">
@@ -1657,23 +2398,23 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="23">
-        <v>2</v>
-      </c>
-      <c r="B23" s="23" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="24" t="s">
+      <c r="C23" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="22" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="1">
@@ -1689,23 +2430,23 @@
         <v>0.91100000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="23">
-        <v>2</v>
-      </c>
-      <c r="B24" s="23" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="24" t="s">
+      <c r="C24" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="22" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="1">
@@ -1721,23 +2462,23 @@
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="23">
-        <v>2</v>
-      </c>
-      <c r="B25" s="23" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="24" t="s">
+      <c r="C25" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="22" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="1">
@@ -1753,23 +2494,23 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="23">
-        <v>2</v>
-      </c>
-      <c r="B26" s="23" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="24" t="s">
+      <c r="C26" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="22" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="1">
@@ -1796,7 +2537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0787812-28CF-4AB7-828B-54F80CCDA331}">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -1804,20 +2545,20 @@
       <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1833,7 +2574,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +2590,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1861,53 +2602,53 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="40"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="24" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding updated NN analysis file
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sensata2com-my.sharepoint.com/personal/sofithcheallaigh_sensata_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4059ED-09FB-483C-A1CC-09561C249FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{DA4059ED-09FB-483C-A1CC-09561C249FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF198DC9-A440-4E5D-8B7F-2CFBC3A3936D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
-    <sheet name="Keras Seq" sheetId="1" r:id="rId2"/>
+    <sheet name="ClosedDoor" sheetId="3" r:id="rId1"/>
+    <sheet name="DisplayStand" sheetId="4" r:id="rId2"/>
+    <sheet name="Keras Seq" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="36">
   <si>
     <t xml:space="preserve">Model: </t>
   </si>
@@ -166,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +177,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,28 +857,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -877,40 +911,238 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1276,19 +1508,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9512EAE-7E03-4C9A-9560-62E0DE7C04A5}">
-  <dimension ref="A2:O34"/>
+  <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="88" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1"/>
@@ -1301,10 +1533,10 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="88" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
@@ -1317,10 +1549,10 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="88" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1"/>
@@ -1336,22 +1568,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="49" t="s">
+      <c r="B5" s="90"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="50" t="s">
+      <c r="E5" s="90"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="91"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -1360,34 +1592,34 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="46" t="s">
+      <c r="J6" s="94" t="s">
         <v>10</v>
       </c>
       <c r="N6" t="s">
@@ -1398,35 +1630,35 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
-        <v>2</v>
-      </c>
-      <c r="B7" s="37" t="s">
+      <c r="A7" s="96">
+        <v>2</v>
+      </c>
+      <c r="B7" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="21">
-        <v>20</v>
-      </c>
-      <c r="H7" s="43">
+      <c r="D7" s="99" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="98" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="101">
+        <v>10</v>
+      </c>
+      <c r="H7" s="100">
         <v>32</v>
       </c>
-      <c r="I7" s="43">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="J7" s="22">
-        <v>0.18099999999999999</v>
+      <c r="I7" s="100">
+        <v>0.9</v>
+      </c>
+      <c r="J7" s="98">
+        <v>0.16800000000000001</v>
       </c>
       <c r="N7" t="s">
         <v>31</v>
@@ -1435,7 +1667,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
         <v>3</v>
       </c>
@@ -1445,7 +1677,7 @@
       <c r="C8" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="47" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="38" t="s">
@@ -1454,49 +1686,49 @@
       <c r="F8" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="32">
-        <v>20</v>
+      <c r="G8" s="48">
+        <v>10</v>
       </c>
       <c r="H8" s="38">
         <v>32</v>
       </c>
       <c r="I8" s="38">
-        <v>0.79900000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="J8" s="33">
-        <v>0.38800000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <v>2</v>
-      </c>
-      <c r="B9" s="39" t="s">
+      <c r="A9" s="20">
+        <v>2</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="1">
-        <v>30</v>
-      </c>
-      <c r="H9" s="41">
+      <c r="D9" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="21">
+        <v>20</v>
+      </c>
+      <c r="H9" s="43">
         <v>32</v>
       </c>
-      <c r="I9" s="41">
-        <v>0.748</v>
-      </c>
-      <c r="J9" s="19">
-        <v>0.47199999999999998</v>
+      <c r="I9" s="43">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="J9" s="22">
+        <v>0.18099999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1519,244 +1751,244 @@
         <v>28</v>
       </c>
       <c r="G10" s="32">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H10" s="38">
         <v>32</v>
       </c>
       <c r="I10" s="38">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="J10" s="33">
+        <v>0.38800000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>2</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1">
+        <v>30</v>
+      </c>
+      <c r="H11" s="41">
+        <v>32</v>
+      </c>
+      <c r="I11" s="41">
+        <v>0.748</v>
+      </c>
+      <c r="J11" s="19">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="86">
+        <v>3</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="87">
+        <v>30</v>
+      </c>
+      <c r="H12" s="63">
+        <v>32</v>
+      </c>
+      <c r="I12" s="63">
         <v>0.999</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J12" s="64">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="34">
-        <v>2</v>
-      </c>
-      <c r="B11" s="40" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
+        <v>2</v>
+      </c>
+      <c r="B13" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C13" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="35">
+      <c r="D13" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="35">
         <v>40</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H13" s="40">
         <v>32</v>
       </c>
-      <c r="I11" s="40">
+      <c r="I13" s="40">
         <v>0.1</v>
       </c>
-      <c r="J11" s="36">
+      <c r="J13" s="36">
         <v>2.3029999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
         <v>3</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B14" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C14" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="32">
+      <c r="D14" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="32">
         <v>40</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H14" s="38">
         <v>32</v>
       </c>
-      <c r="I12" s="38">
+      <c r="I14" s="38">
         <v>0.8</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J14" s="33">
         <v>0.33200000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <v>2</v>
-      </c>
-      <c r="B13" s="41" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>2</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="D15" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="1">
         <v>50</v>
       </c>
-      <c r="H13" s="41">
+      <c r="H15" s="41">
         <v>32</v>
       </c>
-      <c r="I13" s="41">
+      <c r="I15" s="41">
         <v>0.1</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J15" s="19">
         <v>2.3029999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="84">
         <v>3</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B16" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C16" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="D16" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="85">
         <v>50</v>
       </c>
-      <c r="H14" s="42">
+      <c r="H16" s="73">
         <v>32</v>
       </c>
-      <c r="I14" s="42">
+      <c r="I16" s="73">
         <v>0.99</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J16" s="74">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
-        <v>2</v>
-      </c>
-      <c r="B15" s="37" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>2</v>
+      </c>
+      <c r="B17" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="29">
+      <c r="D17" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="29">
         <v>10</v>
       </c>
-      <c r="H15" s="43">
+      <c r="H17" s="43">
         <v>64</v>
       </c>
-      <c r="I15" s="43">
+      <c r="I17" s="43">
         <v>0.67900000000000005</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J17" s="22">
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="31">
-        <v>3</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="60">
-        <v>10</v>
-      </c>
-      <c r="H16" s="38">
-        <v>64</v>
-      </c>
-      <c r="I16" s="38">
-        <v>0.79900000000000004</v>
-      </c>
-      <c r="J16" s="33">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="34">
-        <v>2</v>
-      </c>
-      <c r="B17" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="63">
-        <v>20</v>
-      </c>
-      <c r="H17" s="40">
-        <v>64</v>
-      </c>
-      <c r="I17" s="40">
-        <v>0.67800000000000005</v>
-      </c>
-      <c r="J17" s="36">
-        <v>0.51400000000000001</v>
-      </c>
-    </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="59">
+      <c r="A18" s="31">
         <v>3</v>
       </c>
       <c r="B18" s="38" t="s">
@@ -1765,7 +1997,7 @@
       <c r="C18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="47" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="38" t="s">
@@ -1774,30 +2006,30 @@
       <c r="F18" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="60">
-        <v>20</v>
+      <c r="G18" s="48">
+        <v>10</v>
       </c>
       <c r="H18" s="38">
         <v>64</v>
       </c>
       <c r="I18" s="38">
-        <v>0.998</v>
+        <v>0.79900000000000004</v>
       </c>
       <c r="J18" s="33">
-        <v>7.0000000000000001E-3</v>
+        <v>0.33900000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="34">
         <v>2</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="49" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="50" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="40" t="s">
@@ -1806,21 +2038,21 @@
       <c r="F19" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="63">
-        <v>30</v>
+      <c r="G19" s="51">
+        <v>20</v>
       </c>
       <c r="H19" s="40">
         <v>64</v>
       </c>
       <c r="I19" s="40">
-        <v>0.91</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="J19" s="36">
-        <v>0.14099999999999999</v>
+        <v>0.51400000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="59">
+      <c r="A20" s="47">
         <v>3</v>
       </c>
       <c r="B20" s="38" t="s">
@@ -1829,7 +2061,7 @@
       <c r="C20" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="47" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="38" t="s">
@@ -1838,245 +2070,245 @@
       <c r="F20" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="60">
-        <v>30</v>
+      <c r="G20" s="48">
+        <v>20</v>
       </c>
       <c r="H20" s="38">
         <v>64</v>
       </c>
       <c r="I20" s="38">
+        <v>0.998</v>
+      </c>
+      <c r="J20" s="33">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="76">
+        <v>2</v>
+      </c>
+      <c r="B21" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="79" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="82">
+        <v>30</v>
+      </c>
+      <c r="H21" s="80">
+        <v>64</v>
+      </c>
+      <c r="I21" s="80">
+        <v>0.91</v>
+      </c>
+      <c r="J21" s="78">
+        <v>0.14099999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="62">
+        <v>3</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="83">
+        <v>30</v>
+      </c>
+      <c r="H22" s="63">
+        <v>64</v>
+      </c>
+      <c r="I22" s="63">
         <v>0.99399999999999999</v>
       </c>
-      <c r="J20" s="33">
+      <c r="J22" s="64">
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="34">
-        <v>2</v>
-      </c>
-      <c r="B21" s="61" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="76">
+        <v>2</v>
+      </c>
+      <c r="B23" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C23" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="63">
+      <c r="D23" s="79" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="82">
         <v>40</v>
       </c>
-      <c r="H21" s="40">
+      <c r="H23" s="80">
         <v>64</v>
       </c>
-      <c r="I21" s="40">
+      <c r="I23" s="80">
         <v>0.999</v>
       </c>
-      <c r="J21" s="36">
+      <c r="J23" s="78">
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="59">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="47">
         <v>3</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B24" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C24" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="60">
+      <c r="D24" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="48">
         <v>40</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H24" s="38">
         <v>64</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I24" s="38">
         <v>0.8</v>
       </c>
-      <c r="J22" s="33">
+      <c r="J24" s="33">
         <v>0.33200000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
-        <v>2</v>
-      </c>
-      <c r="B23" s="39" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>2</v>
+      </c>
+      <c r="B25" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C25" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="57" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="17">
+      <c r="D25" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="17">
         <v>50</v>
       </c>
-      <c r="H23" s="41">
+      <c r="H25" s="41">
         <v>64</v>
       </c>
-      <c r="I23" s="41">
+      <c r="I25" s="41">
         <v>0.75700000000000001</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J25" s="19">
         <v>0.46400000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="58">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="46">
         <v>3</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B26" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="5">
+      <c r="D26" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="5">
         <v>50</v>
       </c>
-      <c r="H24" s="42">
+      <c r="H26" s="42">
         <v>64</v>
       </c>
-      <c r="I24" s="42">
+      <c r="I26" s="42">
         <v>0.79900000000000004</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J26" s="4">
         <v>0.33200000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
-        <v>2</v>
-      </c>
-      <c r="B25" s="37" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
+        <v>2</v>
+      </c>
+      <c r="B27" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C27" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="48">
+      <c r="D27" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="44">
         <v>10</v>
       </c>
-      <c r="H25" s="64">
+      <c r="H27" s="52">
         <v>128</v>
       </c>
-      <c r="I25" s="48">
+      <c r="I27" s="44">
         <v>0.90500000000000003</v>
       </c>
-      <c r="J25" s="22">
+      <c r="J27" s="22">
         <v>0.106</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="59">
-        <v>3</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="59">
-        <v>10</v>
-      </c>
-      <c r="H26" s="65">
-        <v>128</v>
-      </c>
-      <c r="I26" s="59">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="J26" s="33">
-        <v>2.3029999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="34">
-        <v>2</v>
-      </c>
-      <c r="B27" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="62">
-        <v>20</v>
-      </c>
-      <c r="H27" s="66">
-        <v>128</v>
-      </c>
-      <c r="I27" s="62">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="J27" s="36">
-        <v>0.52600000000000002</v>
-      </c>
-    </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="59">
+      <c r="A28" s="47">
         <v>3</v>
       </c>
       <c r="B28" s="38" t="s">
@@ -2085,7 +2317,7 @@
       <c r="C28" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="59" t="s">
+      <c r="D28" s="47" t="s">
         <v>24</v>
       </c>
       <c r="E28" s="38" t="s">
@@ -2094,30 +2326,30 @@
       <c r="F28" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="59">
-        <v>20</v>
-      </c>
-      <c r="H28" s="65">
+      <c r="G28" s="47">
+        <v>10</v>
+      </c>
+      <c r="H28" s="53">
         <v>128</v>
       </c>
-      <c r="I28" s="59">
-        <v>0.99399999999999999</v>
+      <c r="I28" s="47">
+        <v>0.10100000000000001</v>
       </c>
       <c r="J28" s="33">
-        <v>2.1999999999999999E-2</v>
+        <v>2.3029999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="34">
         <v>2</v>
       </c>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="49" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="62" t="s">
+      <c r="D29" s="50" t="s">
         <v>24</v>
       </c>
       <c r="E29" s="40" t="s">
@@ -2126,81 +2358,85 @@
       <c r="F29" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="G29" s="62">
-        <v>30</v>
-      </c>
-      <c r="H29" s="66">
+      <c r="G29" s="50">
+        <v>20</v>
+      </c>
+      <c r="H29" s="54">
         <v>128</v>
       </c>
-      <c r="I29" s="62">
-        <v>0.95799999999999996</v>
+      <c r="I29" s="50">
+        <v>0.69899999999999995</v>
       </c>
       <c r="J29" s="36">
-        <v>0.128</v>
+        <v>0.52600000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="59">
+      <c r="A30" s="62">
         <v>3</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="59">
-        <v>30</v>
+      <c r="D30" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="62">
+        <v>20</v>
       </c>
       <c r="H30" s="65">
         <v>128</v>
       </c>
-      <c r="I30" s="59">
-        <v>0.1</v>
-      </c>
-      <c r="J30" s="33">
-        <v>0</v>
+      <c r="I30" s="62">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J30" s="64">
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="34">
-        <v>2</v>
-      </c>
-      <c r="B31" s="61" t="s">
+      <c r="A31" s="76">
+        <v>2</v>
+      </c>
+      <c r="B31" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="62">
-        <v>40</v>
-      </c>
-      <c r="H31" s="66">
+      <c r="D31" s="79" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="79">
+        <v>30</v>
+      </c>
+      <c r="H31" s="81">
         <v>128</v>
       </c>
-      <c r="I31" s="62"/>
-      <c r="J31" s="36"/>
+      <c r="I31" s="79">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="J31" s="78">
+        <v>0.128</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="59">
+      <c r="A32" s="47">
         <v>3</v>
       </c>
       <c r="B32" s="38" t="s">
@@ -2209,7 +2445,7 @@
       <c r="C32" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="59" t="s">
+      <c r="D32" s="47" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="38" t="s">
@@ -2218,70 +2454,466 @@
       <c r="F32" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="59">
+      <c r="G32" s="47">
+        <v>30</v>
+      </c>
+      <c r="H32" s="53">
+        <v>128</v>
+      </c>
+      <c r="I32" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="J32" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="34">
+        <v>2</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="50">
         <v>40</v>
       </c>
-      <c r="H32" s="65">
+      <c r="H33" s="54">
         <v>128</v>
       </c>
-      <c r="I32" s="59"/>
-      <c r="J32" s="33"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
-        <v>2</v>
-      </c>
-      <c r="B33" s="39" t="s">
+      <c r="I33" s="50">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="J33" s="36">
+        <v>0.48699999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="47">
+        <v>3</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="47">
+        <v>40</v>
+      </c>
+      <c r="H34" s="53">
+        <v>128</v>
+      </c>
+      <c r="I34" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="J34" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="66">
+        <v>2</v>
+      </c>
+      <c r="B35" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C35" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="57" t="s">
-        <v>24</v>
-      </c>
-      <c r="E33" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G33" s="57">
+      <c r="D35" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="69">
         <v>50</v>
       </c>
-      <c r="H33" s="67">
+      <c r="H35" s="71">
         <v>128</v>
       </c>
-      <c r="I33" s="57"/>
-      <c r="J33" s="19"/>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="58">
+      <c r="I35" s="69">
+        <v>0.91</v>
+      </c>
+      <c r="J35" s="68">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="72">
         <v>3</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B36" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C36" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" s="58">
+      <c r="D36" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="72">
         <v>50</v>
       </c>
-      <c r="H34" s="68">
+      <c r="H36" s="75">
         <v>128</v>
       </c>
-      <c r="I34" s="58"/>
-      <c r="J34" s="4"/>
+      <c r="I36" s="72">
+        <v>0.998</v>
+      </c>
+      <c r="J36" s="74">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="20">
+        <v>2</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="44">
+        <v>10</v>
+      </c>
+      <c r="H37" s="52">
+        <v>256</v>
+      </c>
+      <c r="I37" s="44">
+        <v>0.65</v>
+      </c>
+      <c r="J37" s="22">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="47">
+        <v>3</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="47">
+        <v>10</v>
+      </c>
+      <c r="H38" s="53">
+        <v>256</v>
+      </c>
+      <c r="I38" s="47">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="J38" s="33">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="34">
+        <v>2</v>
+      </c>
+      <c r="B39" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="50">
+        <v>20</v>
+      </c>
+      <c r="H39" s="54">
+        <v>256</v>
+      </c>
+      <c r="I39" s="50">
+        <v>0.871</v>
+      </c>
+      <c r="J39" s="36">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="62">
+        <v>3</v>
+      </c>
+      <c r="B40" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="62">
+        <v>20</v>
+      </c>
+      <c r="H40" s="65">
+        <v>256</v>
+      </c>
+      <c r="I40" s="62">
+        <v>0.998</v>
+      </c>
+      <c r="J40" s="64">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="34">
+        <v>2</v>
+      </c>
+      <c r="B41" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="50">
+        <v>30</v>
+      </c>
+      <c r="H41" s="54">
+        <v>256</v>
+      </c>
+      <c r="I41" s="50">
+        <v>0.871</v>
+      </c>
+      <c r="J41" s="36">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="62">
+        <v>3</v>
+      </c>
+      <c r="B42" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="62">
+        <v>30</v>
+      </c>
+      <c r="H42" s="65">
+        <v>256</v>
+      </c>
+      <c r="I42" s="62">
+        <v>0.998</v>
+      </c>
+      <c r="J42" s="64">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="34">
+        <v>2</v>
+      </c>
+      <c r="B43" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="50">
+        <v>40</v>
+      </c>
+      <c r="H43" s="54">
+        <v>256</v>
+      </c>
+      <c r="I43" s="50">
+        <v>0.98</v>
+      </c>
+      <c r="J43" s="36">
+        <v>0.13100000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="47">
+        <v>3</v>
+      </c>
+      <c r="B44" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="47">
+        <v>40</v>
+      </c>
+      <c r="H44" s="53">
+        <v>256</v>
+      </c>
+      <c r="I44" s="47">
+        <v>0.999</v>
+      </c>
+      <c r="J44" s="33">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
+        <v>2</v>
+      </c>
+      <c r="B45" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="45">
+        <v>50</v>
+      </c>
+      <c r="H45" s="55">
+        <v>256</v>
+      </c>
+      <c r="I45" s="45">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="J45" s="19">
+        <v>2.3029999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="46">
+        <v>3</v>
+      </c>
+      <c r="B46" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="46">
+        <v>50</v>
+      </c>
+      <c r="H46" s="56">
+        <v>256</v>
+      </c>
+      <c r="I46" s="46">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="J46" s="4">
+        <v>0.56200000000000006</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2295,6 +2927,1290 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3EA1287-235E-4BCC-86D0-1A585A75401B}">
+  <dimension ref="A2:O46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="88" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="90"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="90"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="91"/>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="102">
+        <v>2</v>
+      </c>
+      <c r="B7" s="103" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="107">
+        <v>10</v>
+      </c>
+      <c r="H7" s="106">
+        <v>32</v>
+      </c>
+      <c r="I7" s="106">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="J7" s="104">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="108">
+        <v>3</v>
+      </c>
+      <c r="B8" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="112">
+        <v>10</v>
+      </c>
+      <c r="H8" s="109">
+        <v>32</v>
+      </c>
+      <c r="I8" s="109">
+        <v>2E-3</v>
+      </c>
+      <c r="J8" s="110">
+        <v>2.516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="102">
+        <v>2</v>
+      </c>
+      <c r="B9" s="103" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="102" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="113">
+        <v>20</v>
+      </c>
+      <c r="H9" s="106">
+        <v>32</v>
+      </c>
+      <c r="I9" s="106">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="J9" s="104">
+        <v>0.91800000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="108">
+        <v>3</v>
+      </c>
+      <c r="B10" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="108" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="114">
+        <v>20</v>
+      </c>
+      <c r="H10" s="109">
+        <v>32</v>
+      </c>
+      <c r="I10" s="109">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="J10" s="110">
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="115">
+        <v>2</v>
+      </c>
+      <c r="B11" s="116" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="118" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="117" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="119">
+        <v>30</v>
+      </c>
+      <c r="H11" s="118">
+        <v>32</v>
+      </c>
+      <c r="I11" s="118">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="J11" s="117">
+        <v>2.3029999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="108">
+        <v>3</v>
+      </c>
+      <c r="B12" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="108" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="114">
+        <v>30</v>
+      </c>
+      <c r="H12" s="109">
+        <v>32</v>
+      </c>
+      <c r="I12" s="109">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="J12" s="110">
+        <v>0.40600000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="120">
+        <v>2</v>
+      </c>
+      <c r="B13" s="121" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="123">
+        <v>40</v>
+      </c>
+      <c r="H13" s="121">
+        <v>32</v>
+      </c>
+      <c r="I13" s="121"/>
+      <c r="J13" s="122"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="108">
+        <v>3</v>
+      </c>
+      <c r="B14" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="108" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="114">
+        <v>40</v>
+      </c>
+      <c r="H14" s="109">
+        <v>32</v>
+      </c>
+      <c r="I14" s="109"/>
+      <c r="J14" s="110"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="115">
+        <v>2</v>
+      </c>
+      <c r="B15" s="118" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="118" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="117" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="119">
+        <v>50</v>
+      </c>
+      <c r="H15" s="118">
+        <v>32</v>
+      </c>
+      <c r="I15" s="118"/>
+      <c r="J15" s="117"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="124">
+        <v>3</v>
+      </c>
+      <c r="B16" s="125" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="126" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="124" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="125" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="126" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="127">
+        <v>50</v>
+      </c>
+      <c r="H16" s="125">
+        <v>32</v>
+      </c>
+      <c r="I16" s="125"/>
+      <c r="J16" s="126"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="102">
+        <v>2</v>
+      </c>
+      <c r="B17" s="103" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="107">
+        <v>10</v>
+      </c>
+      <c r="H17" s="106">
+        <v>64</v>
+      </c>
+      <c r="I17" s="106"/>
+      <c r="J17" s="104"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="108">
+        <v>3</v>
+      </c>
+      <c r="B18" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="112">
+        <v>10</v>
+      </c>
+      <c r="H18" s="109">
+        <v>64</v>
+      </c>
+      <c r="I18" s="109"/>
+      <c r="J18" s="110"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="120">
+        <v>2</v>
+      </c>
+      <c r="B19" s="128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="130">
+        <v>20</v>
+      </c>
+      <c r="H19" s="121">
+        <v>64</v>
+      </c>
+      <c r="I19" s="121"/>
+      <c r="J19" s="122"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="111">
+        <v>3</v>
+      </c>
+      <c r="B20" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="112">
+        <v>20</v>
+      </c>
+      <c r="H20" s="109">
+        <v>64</v>
+      </c>
+      <c r="I20" s="109"/>
+      <c r="J20" s="110"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="120">
+        <v>2</v>
+      </c>
+      <c r="B21" s="128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="130">
+        <v>30</v>
+      </c>
+      <c r="H21" s="121">
+        <v>64</v>
+      </c>
+      <c r="I21" s="121"/>
+      <c r="J21" s="122"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="111">
+        <v>3</v>
+      </c>
+      <c r="B22" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="112">
+        <v>30</v>
+      </c>
+      <c r="H22" s="109">
+        <v>64</v>
+      </c>
+      <c r="I22" s="109"/>
+      <c r="J22" s="110"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="120">
+        <v>2</v>
+      </c>
+      <c r="B23" s="128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="130">
+        <v>40</v>
+      </c>
+      <c r="H23" s="121">
+        <v>64</v>
+      </c>
+      <c r="I23" s="121"/>
+      <c r="J23" s="122"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="111">
+        <v>3</v>
+      </c>
+      <c r="B24" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="112">
+        <v>40</v>
+      </c>
+      <c r="H24" s="109">
+        <v>64</v>
+      </c>
+      <c r="I24" s="109"/>
+      <c r="J24" s="110"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="115">
+        <v>2</v>
+      </c>
+      <c r="B25" s="116" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="131" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="118" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="117" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="132">
+        <v>50</v>
+      </c>
+      <c r="H25" s="118">
+        <v>64</v>
+      </c>
+      <c r="I25" s="118"/>
+      <c r="J25" s="117"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="133">
+        <v>3</v>
+      </c>
+      <c r="B26" s="125" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="126" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="125" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="126" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="134">
+        <v>50</v>
+      </c>
+      <c r="H26" s="125">
+        <v>64</v>
+      </c>
+      <c r="I26" s="125"/>
+      <c r="J26" s="126"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="102">
+        <v>2</v>
+      </c>
+      <c r="B27" s="103" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="105">
+        <v>10</v>
+      </c>
+      <c r="H27" s="135">
+        <v>128</v>
+      </c>
+      <c r="I27" s="105"/>
+      <c r="J27" s="104"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="111">
+        <v>3</v>
+      </c>
+      <c r="B28" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="111">
+        <v>10</v>
+      </c>
+      <c r="H28" s="136">
+        <v>128</v>
+      </c>
+      <c r="I28" s="111"/>
+      <c r="J28" s="110"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="120">
+        <v>2</v>
+      </c>
+      <c r="B29" s="128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="129">
+        <v>20</v>
+      </c>
+      <c r="H29" s="137">
+        <v>128</v>
+      </c>
+      <c r="I29" s="129"/>
+      <c r="J29" s="122"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="111">
+        <v>3</v>
+      </c>
+      <c r="B30" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="111">
+        <v>20</v>
+      </c>
+      <c r="H30" s="136">
+        <v>128</v>
+      </c>
+      <c r="I30" s="111"/>
+      <c r="J30" s="110"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="120">
+        <v>2</v>
+      </c>
+      <c r="B31" s="128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="129">
+        <v>30</v>
+      </c>
+      <c r="H31" s="137">
+        <v>128</v>
+      </c>
+      <c r="I31" s="129"/>
+      <c r="J31" s="122"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="111">
+        <v>3</v>
+      </c>
+      <c r="B32" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="111">
+        <v>30</v>
+      </c>
+      <c r="H32" s="136">
+        <v>128</v>
+      </c>
+      <c r="I32" s="111"/>
+      <c r="J32" s="110"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="120">
+        <v>2</v>
+      </c>
+      <c r="B33" s="128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="129">
+        <v>40</v>
+      </c>
+      <c r="H33" s="137">
+        <v>128</v>
+      </c>
+      <c r="I33" s="129"/>
+      <c r="J33" s="122"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="111">
+        <v>3</v>
+      </c>
+      <c r="B34" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="111">
+        <v>40</v>
+      </c>
+      <c r="H34" s="136">
+        <v>128</v>
+      </c>
+      <c r="I34" s="111"/>
+      <c r="J34" s="110"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="115">
+        <v>2</v>
+      </c>
+      <c r="B35" s="116" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="131" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="118" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="117" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="131">
+        <v>50</v>
+      </c>
+      <c r="H35" s="138">
+        <v>128</v>
+      </c>
+      <c r="I35" s="131"/>
+      <c r="J35" s="117"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="133">
+        <v>3</v>
+      </c>
+      <c r="B36" s="125" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="126" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="125" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="126" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="133">
+        <v>50</v>
+      </c>
+      <c r="H36" s="139">
+        <v>128</v>
+      </c>
+      <c r="I36" s="133"/>
+      <c r="J36" s="126"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="102">
+        <v>2</v>
+      </c>
+      <c r="B37" s="103" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="105">
+        <v>10</v>
+      </c>
+      <c r="H37" s="135">
+        <v>256</v>
+      </c>
+      <c r="I37" s="105"/>
+      <c r="J37" s="104"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="111">
+        <v>3</v>
+      </c>
+      <c r="B38" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="111">
+        <v>10</v>
+      </c>
+      <c r="H38" s="136">
+        <v>256</v>
+      </c>
+      <c r="I38" s="111"/>
+      <c r="J38" s="110"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="120">
+        <v>2</v>
+      </c>
+      <c r="B39" s="128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="129">
+        <v>20</v>
+      </c>
+      <c r="H39" s="137">
+        <v>256</v>
+      </c>
+      <c r="I39" s="129"/>
+      <c r="J39" s="122"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="111">
+        <v>3</v>
+      </c>
+      <c r="B40" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="111">
+        <v>20</v>
+      </c>
+      <c r="H40" s="136">
+        <v>256</v>
+      </c>
+      <c r="I40" s="111"/>
+      <c r="J40" s="110"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="120">
+        <v>2</v>
+      </c>
+      <c r="B41" s="128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="129">
+        <v>30</v>
+      </c>
+      <c r="H41" s="137">
+        <v>256</v>
+      </c>
+      <c r="I41" s="129"/>
+      <c r="J41" s="122"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="111">
+        <v>3</v>
+      </c>
+      <c r="B42" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="111">
+        <v>30</v>
+      </c>
+      <c r="H42" s="136">
+        <v>256</v>
+      </c>
+      <c r="I42" s="111"/>
+      <c r="J42" s="110"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="120">
+        <v>2</v>
+      </c>
+      <c r="B43" s="128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="122" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="122" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="129">
+        <v>40</v>
+      </c>
+      <c r="H43" s="137">
+        <v>256</v>
+      </c>
+      <c r="I43" s="129"/>
+      <c r="J43" s="122"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="111">
+        <v>3</v>
+      </c>
+      <c r="B44" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="110" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="111">
+        <v>40</v>
+      </c>
+      <c r="H44" s="136">
+        <v>256</v>
+      </c>
+      <c r="I44" s="111"/>
+      <c r="J44" s="110"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="115">
+        <v>2</v>
+      </c>
+      <c r="B45" s="116" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="131" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="118" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="117" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="131">
+        <v>50</v>
+      </c>
+      <c r="H45" s="138">
+        <v>256</v>
+      </c>
+      <c r="I45" s="131"/>
+      <c r="J45" s="117"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="133">
+        <v>3</v>
+      </c>
+      <c r="B46" s="125" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="126" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="125" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="126" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="133">
+        <v>50</v>
+      </c>
+      <c r="H46" s="139">
+        <v>256</v>
+      </c>
+      <c r="I46" s="133"/>
+      <c r="J46" s="126"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:J5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCBFCE0-D62A-4787-8AAA-20AB7ACA5ECA}">
   <dimension ref="A1:J26"/>
   <sheetViews>
@@ -2327,22 +4243,22 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55" t="s">
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="53"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="53" t="s">
+      <c r="E4" s="58"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="56"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="61"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">

</xml_diff>

<commit_message>
updating NN results file to include work in SGD
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B103D3-E9E0-49CC-A23D-335905C21954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9AED72-9A60-45D6-9C32-1E3E1341CE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
   <sheets>
     <sheet name="ClosedDoor" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="LargeBin" sheetId="5" r:id="rId3"/>
     <sheet name="StorageBox" sheetId="6" r:id="rId4"/>
     <sheet name="Keras Seq" sheetId="1" r:id="rId5"/>
+    <sheet name="AllData" sheetId="7" r:id="rId6"/>
+    <sheet name="SGD" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="49">
   <si>
     <t xml:space="preserve">Model: </t>
   </si>
@@ -159,6 +161,33 @@
   <si>
     <t>Large Bin</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>model_sgd_1 parameters</t>
+  </si>
+  <si>
+    <t>Image #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#1 </t>
+  </si>
+  <si>
+    <t>mode_sgd_2 parameters</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
 </sst>
 </file>
 
@@ -213,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -736,11 +765,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1043,6 +1137,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1104,6 +1217,343 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>58433</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>86575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69C6FD5F-3E46-3043-1A27-B8EAE75B6424}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7010400" y="514350"/>
+          <a:ext cx="9192908" cy="6087325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A91BD2-C3EE-BFF3-9C84-FF32588FFD15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6629400" y="6657975"/>
+          <a:ext cx="3733800" cy="2647950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>258657</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>167695</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E32A945-CB6A-44F7-E76B-126CAA2DC9B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17221200" y="571500"/>
+          <a:ext cx="10155132" cy="6111295"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9079988A-9870-ACC4-C1EB-58654ED3118A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12363450" y="6629400"/>
+          <a:ext cx="3733800" cy="2647950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{474C290D-F560-4ED8-F48F-3B11F90E22A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6648450" y="9677400"/>
+          <a:ext cx="3733800" cy="2647950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CC1D2FE-1970-E7E3-E530-521F1F8B6D90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12487275" y="9744075"/>
+          <a:ext cx="3733800" cy="2647950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1410,7 +1860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9512EAE-7E03-4C9A-9560-62E0DE7C04A5}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
@@ -2830,7 +3280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3EA1287-235E-4BCC-86D0-1A585A75401B}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
@@ -4250,7 +4700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287FE74C-991A-4067-9EE8-0A2DE1F6D0D7}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
@@ -5670,8 +6120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EA4EDF-FB69-457D-A5E5-9C9DD8D38A58}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7849,4 +8299,1774 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E5A619-FAB5-4BB1-8793-63B61E683A60}">
+  <dimension ref="A2:O46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="94" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="95"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="94" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="95"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="96"/>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="87" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="87" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>2</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="29">
+        <v>10</v>
+      </c>
+      <c r="H7" s="43">
+        <v>32</v>
+      </c>
+      <c r="I7" s="43">
+        <v>0.34</v>
+      </c>
+      <c r="J7" s="22">
+        <v>1.597</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>3</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="48">
+        <v>10</v>
+      </c>
+      <c r="H8" s="38">
+        <v>32</v>
+      </c>
+      <c r="I8" s="38">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="J8" s="33">
+        <v>1.016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
+        <v>2</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="21">
+        <v>20</v>
+      </c>
+      <c r="H9" s="43">
+        <v>32</v>
+      </c>
+      <c r="I9" s="43">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="J9" s="22">
+        <v>1.454</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>3</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="32">
+        <v>20</v>
+      </c>
+      <c r="H10" s="38">
+        <v>32</v>
+      </c>
+      <c r="I10" s="38">
+        <v>0.625</v>
+      </c>
+      <c r="J10" s="33">
+        <v>0.80800000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>2</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1">
+        <v>30</v>
+      </c>
+      <c r="H11" s="41">
+        <v>32</v>
+      </c>
+      <c r="I11" s="41">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="J11" s="19">
+        <v>1.466</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>3</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="32">
+        <v>30</v>
+      </c>
+      <c r="H12" s="38">
+        <v>32</v>
+      </c>
+      <c r="I12" s="38">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="J12" s="33">
+        <v>1.0189999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
+        <v>2</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="35">
+        <v>40</v>
+      </c>
+      <c r="H13" s="40">
+        <v>32</v>
+      </c>
+      <c r="I13" s="40">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="J13" s="36">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
+        <v>3</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="32">
+        <v>40</v>
+      </c>
+      <c r="H14" s="38">
+        <v>32</v>
+      </c>
+      <c r="I14" s="38">
+        <v>0.5151</v>
+      </c>
+      <c r="J14" s="33">
+        <v>1.115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>2</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="1">
+        <v>50</v>
+      </c>
+      <c r="H15" s="41">
+        <v>32</v>
+      </c>
+      <c r="I15" s="41"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="3">
+        <v>50</v>
+      </c>
+      <c r="H16" s="42">
+        <v>32</v>
+      </c>
+      <c r="I16" s="42"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>2</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="29">
+        <v>10</v>
+      </c>
+      <c r="H17" s="43">
+        <v>64</v>
+      </c>
+      <c r="I17" s="43">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="J17" s="22">
+        <v>1.599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
+        <v>3</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="48">
+        <v>10</v>
+      </c>
+      <c r="H18" s="38">
+        <v>64</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="33"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="34">
+        <v>2</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="51">
+        <v>20</v>
+      </c>
+      <c r="H19" s="40">
+        <v>64</v>
+      </c>
+      <c r="I19" s="40"/>
+      <c r="J19" s="36"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="47">
+        <v>3</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="48">
+        <v>20</v>
+      </c>
+      <c r="H20" s="38">
+        <v>64</v>
+      </c>
+      <c r="I20" s="38"/>
+      <c r="J20" s="33"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="34">
+        <v>2</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="51">
+        <v>30</v>
+      </c>
+      <c r="H21" s="40">
+        <v>64</v>
+      </c>
+      <c r="I21" s="40"/>
+      <c r="J21" s="36"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="47">
+        <v>3</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="48">
+        <v>30</v>
+      </c>
+      <c r="H22" s="38">
+        <v>64</v>
+      </c>
+      <c r="I22" s="38"/>
+      <c r="J22" s="33"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="34">
+        <v>2</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="51">
+        <v>40</v>
+      </c>
+      <c r="H23" s="40">
+        <v>64</v>
+      </c>
+      <c r="I23" s="40"/>
+      <c r="J23" s="36"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="47">
+        <v>3</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="48">
+        <v>40</v>
+      </c>
+      <c r="H24" s="38">
+        <v>64</v>
+      </c>
+      <c r="I24" s="38"/>
+      <c r="J24" s="33"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>2</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="17">
+        <v>50</v>
+      </c>
+      <c r="H25" s="41">
+        <v>64</v>
+      </c>
+      <c r="I25" s="41"/>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="46">
+        <v>3</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="5">
+        <v>50</v>
+      </c>
+      <c r="H26" s="42">
+        <v>64</v>
+      </c>
+      <c r="I26" s="42"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
+        <v>2</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="44">
+        <v>10</v>
+      </c>
+      <c r="H27" s="52">
+        <v>128</v>
+      </c>
+      <c r="I27" s="44"/>
+      <c r="J27" s="22"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="47">
+        <v>3</v>
+      </c>
+      <c r="B28" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="47">
+        <v>10</v>
+      </c>
+      <c r="H28" s="53">
+        <v>128</v>
+      </c>
+      <c r="I28" s="47"/>
+      <c r="J28" s="33"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="34">
+        <v>2</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="50">
+        <v>20</v>
+      </c>
+      <c r="H29" s="54">
+        <v>128</v>
+      </c>
+      <c r="I29" s="50"/>
+      <c r="J29" s="36"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="47">
+        <v>3</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="47">
+        <v>20</v>
+      </c>
+      <c r="H30" s="53">
+        <v>128</v>
+      </c>
+      <c r="I30" s="47"/>
+      <c r="J30" s="33"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="34">
+        <v>2</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="50">
+        <v>30</v>
+      </c>
+      <c r="H31" s="54">
+        <v>128</v>
+      </c>
+      <c r="I31" s="50"/>
+      <c r="J31" s="36"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="47">
+        <v>3</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="47">
+        <v>30</v>
+      </c>
+      <c r="H32" s="53">
+        <v>128</v>
+      </c>
+      <c r="I32" s="47"/>
+      <c r="J32" s="33"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="34">
+        <v>2</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="50">
+        <v>40</v>
+      </c>
+      <c r="H33" s="54">
+        <v>128</v>
+      </c>
+      <c r="I33" s="50"/>
+      <c r="J33" s="36"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="47">
+        <v>3</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="47">
+        <v>40</v>
+      </c>
+      <c r="H34" s="53">
+        <v>128</v>
+      </c>
+      <c r="I34" s="47"/>
+      <c r="J34" s="33"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="16">
+        <v>2</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="45">
+        <v>50</v>
+      </c>
+      <c r="H35" s="55">
+        <v>128</v>
+      </c>
+      <c r="I35" s="45"/>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="46">
+        <v>3</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="46">
+        <v>50</v>
+      </c>
+      <c r="H36" s="56">
+        <v>128</v>
+      </c>
+      <c r="I36" s="46"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="20">
+        <v>2</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="44">
+        <v>10</v>
+      </c>
+      <c r="H37" s="52">
+        <v>256</v>
+      </c>
+      <c r="I37" s="44"/>
+      <c r="J37" s="22"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="47">
+        <v>3</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="47">
+        <v>10</v>
+      </c>
+      <c r="H38" s="53">
+        <v>256</v>
+      </c>
+      <c r="I38" s="47"/>
+      <c r="J38" s="33"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="34">
+        <v>2</v>
+      </c>
+      <c r="B39" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="50">
+        <v>20</v>
+      </c>
+      <c r="H39" s="54">
+        <v>256</v>
+      </c>
+      <c r="I39" s="50"/>
+      <c r="J39" s="36"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="47">
+        <v>3</v>
+      </c>
+      <c r="B40" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="47">
+        <v>20</v>
+      </c>
+      <c r="H40" s="53">
+        <v>256</v>
+      </c>
+      <c r="I40" s="47"/>
+      <c r="J40" s="33"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="34">
+        <v>2</v>
+      </c>
+      <c r="B41" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="50">
+        <v>30</v>
+      </c>
+      <c r="H41" s="54">
+        <v>256</v>
+      </c>
+      <c r="I41" s="50"/>
+      <c r="J41" s="36"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="47">
+        <v>3</v>
+      </c>
+      <c r="B42" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="47">
+        <v>30</v>
+      </c>
+      <c r="H42" s="53">
+        <v>256</v>
+      </c>
+      <c r="I42" s="47"/>
+      <c r="J42" s="33"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="34">
+        <v>2</v>
+      </c>
+      <c r="B43" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="50">
+        <v>40</v>
+      </c>
+      <c r="H43" s="54">
+        <v>256</v>
+      </c>
+      <c r="I43" s="50"/>
+      <c r="J43" s="36"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="47">
+        <v>3</v>
+      </c>
+      <c r="B44" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="47">
+        <v>40</v>
+      </c>
+      <c r="H44" s="53">
+        <v>256</v>
+      </c>
+      <c r="I44" s="47"/>
+      <c r="J44" s="33"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
+        <v>2</v>
+      </c>
+      <c r="B45" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="45">
+        <v>50</v>
+      </c>
+      <c r="H45" s="55">
+        <v>256</v>
+      </c>
+      <c r="I45" s="45"/>
+      <c r="J45" s="19"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="46">
+        <v>3</v>
+      </c>
+      <c r="B46" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="46">
+        <v>50</v>
+      </c>
+      <c r="H46" s="56">
+        <v>256</v>
+      </c>
+      <c r="I46" s="46"/>
+      <c r="J46" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:J5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F479D5BE-6F44-4838-BE09-A70623EA1687}">
+  <dimension ref="A2:AC51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="94" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="95"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="94" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="95"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="103"/>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="87" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="87" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="106" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>2</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="29">
+        <v>10</v>
+      </c>
+      <c r="H7" s="43">
+        <v>32</v>
+      </c>
+      <c r="I7" s="43">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="J7" s="22">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="K7" s="104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>3</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="48">
+        <v>10</v>
+      </c>
+      <c r="H8" s="38">
+        <v>32</v>
+      </c>
+      <c r="I8" s="38">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="J8" s="33">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="K8" s="107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>2</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="108">
+        <v>20</v>
+      </c>
+      <c r="H9" s="41">
+        <v>32</v>
+      </c>
+      <c r="I9" s="41">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="J9" s="19">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="K9" s="104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>3</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="32">
+        <v>20</v>
+      </c>
+      <c r="H10" s="38">
+        <v>32</v>
+      </c>
+      <c r="I10" s="38">
+        <v>0.97</v>
+      </c>
+      <c r="J10" s="33">
+        <v>0.109</v>
+      </c>
+      <c r="K10" s="107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>2</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1">
+        <v>30</v>
+      </c>
+      <c r="H11" s="41">
+        <v>32</v>
+      </c>
+      <c r="I11" s="41"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="104"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>3</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="32">
+        <v>30</v>
+      </c>
+      <c r="H12" s="38">
+        <v>32</v>
+      </c>
+      <c r="I12" s="38"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="107"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
+        <v>2</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="35">
+        <v>40</v>
+      </c>
+      <c r="H13" s="40">
+        <v>32</v>
+      </c>
+      <c r="I13" s="40"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="104"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
+        <v>3</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="32">
+        <v>40</v>
+      </c>
+      <c r="H14" s="38">
+        <v>32</v>
+      </c>
+      <c r="I14" s="38"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="107"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>2</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="1">
+        <v>50</v>
+      </c>
+      <c r="H15" s="41">
+        <v>32</v>
+      </c>
+      <c r="I15" s="41"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="104"/>
+    </row>
+    <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="3">
+        <v>50</v>
+      </c>
+      <c r="H16" s="42">
+        <v>32</v>
+      </c>
+      <c r="I16" s="42"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="105"/>
+    </row>
+    <row r="36" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="L36" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="U36" s="102" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="12:22" x14ac:dyDescent="0.25">
+      <c r="L51" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="V51" s="102" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:J5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding u[dated NN results file
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD48DB23-AA9C-4801-8B88-E46F28072366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F20B590-25ED-48E9-9603-A8885F46B4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="55">
   <si>
     <t xml:space="preserve">Model: </t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>#9</t>
+  </si>
+  <si>
+    <t>#10</t>
   </si>
 </sst>
 </file>
@@ -1875,6 +1878,67 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B228E5BC-63BD-B91E-668F-21C9DEC95289}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12830175" y="19078575"/>
+          <a:ext cx="3733800" cy="2647950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6437,8 +6501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EA4EDF-FB69-457D-A5E5-9C9DD8D38A58}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J16"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9920,8 +9984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F479D5BE-6F44-4838-BE09-A70623EA1687}">
   <dimension ref="A2:AC100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10357,7 +10421,9 @@
       <c r="J15" s="19">
         <v>0.751</v>
       </c>
-      <c r="K15" s="96"/>
+      <c r="K15" s="96">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
@@ -10384,9 +10450,15 @@
       <c r="H16" s="42">
         <v>32</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="97"/>
+      <c r="I16" s="42">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="K16" s="97">
+        <v>10</v>
+      </c>
     </row>
     <row r="36" spans="12:21" x14ac:dyDescent="0.25">
       <c r="L36" s="94" t="s">
@@ -10420,9 +10492,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M100" s="94" t="s">
         <v>53</v>
+      </c>
+      <c r="W100" s="94" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating NN analysis folder for sub-dataset analysis
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4548083E-77BE-493F-8F83-932B9183EA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB42F8FD-0F39-4588-A02E-B759643487C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
   <sheets>
     <sheet name="ClosedDoor" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="StorageBox" sheetId="6" r:id="rId4"/>
     <sheet name="AllData - Adam" sheetId="7" r:id="rId5"/>
     <sheet name="AssData - SGD" sheetId="8" r:id="rId6"/>
-    <sheet name="Keras Seq" sheetId="1" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
+    <sheet name="Keras Seq" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="87">
   <si>
     <t xml:space="preserve">Model: </t>
   </si>
@@ -292,6 +293,15 @@
   </si>
   <si>
     <t>#40</t>
+  </si>
+  <si>
+    <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>Optmiser</t>
   </si>
 </sst>
 </file>
@@ -3837,6 +3847,238 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>438892</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95613</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE233A4B-E921-87BC-3BE2-364B048B631D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9753600" y="190500"/>
+          <a:ext cx="5315692" cy="2600688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCE53CCF-797A-1D6C-37C1-E881D127FA97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9772650" y="3457575"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0687A88-422E-8F28-1B3E-2795D3A1CB8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9772650" y="8220075"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F1FD1C1-1B25-6AB9-1AE9-55FFABA08116}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9772650" y="12982575"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -9861,7 +10103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E5A619-FAB5-4BB1-8793-63B61E683A60}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -11225,8 +11467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F479D5BE-6F44-4838-BE09-A70623EA1687}">
   <dimension ref="A2:BY116"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13822,6 +14064,222 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546EE643-96AE-406E-920D-B005CB201B4A}">
+  <dimension ref="A3:P68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="114"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="85" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="113" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="114"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="114" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="95"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="85" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="87" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="87" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="98" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="48">
+        <v>10</v>
+      </c>
+      <c r="I6" s="38">
+        <v>32</v>
+      </c>
+      <c r="J6" s="38">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="K6" s="33">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L6" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>3</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="48">
+        <v>50</v>
+      </c>
+      <c r="I7" s="38">
+        <v>32</v>
+      </c>
+      <c r="J7" s="38">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="K7" s="33">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="L7" s="99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>3</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="48">
+        <v>100</v>
+      </c>
+      <c r="I8" s="38">
+        <v>32</v>
+      </c>
+      <c r="J8" s="38">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="K8" s="33">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="L8" s="99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P68" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:K4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCBFCE0-D62A-4787-8AAA-20AB7ACA5ECA}">
   <dimension ref="A1:J26"/>
   <sheetViews>

</xml_diff>

<commit_message>
updating NN analysis for a reduced dataset
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB42F8FD-0F39-4588-A02E-B759643487C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A0595C-7009-4BB2-BD5B-705053813CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="87">
   <si>
     <t xml:space="preserve">Model: </t>
   </si>
@@ -357,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -945,11 +945,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1291,6 +1386,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4072,6 +4188,860 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D1E71AD-0F5F-6F66-87F3-23A8759D2C62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10182225" y="22602825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC8692F8-83C4-1AF1-55B4-36D492066A36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10001250" y="17745075"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00750CA1-EC4B-1CC7-7C90-F412E4AE087D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10001250" y="27460575"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01C56D03-0F7F-2E54-CB42-35ACA6055735}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10001250" y="32413575"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{600F2685-BB17-C094-7420-6DCD7922AAB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10001250" y="37366575"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>221</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>243</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{826A950B-CFDD-B6A6-8EBB-2FBEDBD57279}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10001250" y="42129075"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9502938A-5894-3148-41FB-8A5793980FC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10001250" y="46891575"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC1E3A46-D224-06E8-173E-1C4875AF7B5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16706850" y="46901100"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>221</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>243</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD691DA9-DE64-4F70-5FD2-B2C14040EEE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16706850" y="42138600"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AF7129B-AF09-25EB-923D-D5B25AF76449}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16706850" y="37376100"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{024C72F5-2AB9-680E-7A53-67D921DE9242}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16706850" y="32423100"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3466B98D-7A37-411B-539A-CC9C04485A5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16706850" y="27470100"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F88A821-C71B-2A03-E616-B53B8369866B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16716375" y="22688550"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F58131B-2A14-552A-ABBE-46938E6B1D5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16706850" y="17754600"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -14065,14 +15035,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546EE643-96AE-406E-920D-B005CB201B4A}">
-  <dimension ref="A3:P68"/>
+  <dimension ref="A3:AA246"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="G99" workbookViewId="0">
+      <selection activeCell="AA94" sqref="AA94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
@@ -14140,40 +15111,40 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
+      <c r="A6" s="121">
         <v>3</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="124">
         <v>0.1</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="125" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="48">
+      <c r="F6" s="122" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="123" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="126">
         <v>10</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="122">
         <v>32</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6" s="122">
         <v>0.85799999999999998</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="123">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L6" s="99">
+      <c r="L6" s="127">
         <v>1</v>
       </c>
     </row>
@@ -14253,9 +15224,644 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
+        <v>3</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="48">
+        <v>150</v>
+      </c>
+      <c r="I9" s="38">
+        <v>32</v>
+      </c>
+      <c r="J9" s="38">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="K9" s="33">
+        <v>0.159</v>
+      </c>
+      <c r="L9" s="99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>3</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="48">
+        <v>200</v>
+      </c>
+      <c r="I10" s="38">
+        <v>32</v>
+      </c>
+      <c r="J10" s="38">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="K10" s="33">
+        <v>0.222</v>
+      </c>
+      <c r="L10" s="99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="31">
+        <v>3</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="48">
+        <v>250</v>
+      </c>
+      <c r="I11" s="38">
+        <v>32</v>
+      </c>
+      <c r="J11" s="38">
+        <v>0.873</v>
+      </c>
+      <c r="K11" s="33">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="L11" s="99">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>3</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="48">
+        <v>300</v>
+      </c>
+      <c r="I12" s="38">
+        <v>32</v>
+      </c>
+      <c r="J12" s="38">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="K12" s="33">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L12" s="99">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
+        <v>3</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="48">
+        <v>350</v>
+      </c>
+      <c r="I13" s="38">
+        <v>32</v>
+      </c>
+      <c r="J13" s="38">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K13" s="33">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="L13" s="99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
+        <v>3</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="48">
+        <v>400</v>
+      </c>
+      <c r="I14" s="38">
+        <v>32</v>
+      </c>
+      <c r="J14" s="38">
+        <v>0.95</v>
+      </c>
+      <c r="K14" s="33">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="L14" s="99">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="5">
+        <v>450</v>
+      </c>
+      <c r="I15" s="42">
+        <v>32</v>
+      </c>
+      <c r="J15" s="42">
+        <v>0.96</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0.311</v>
+      </c>
+      <c r="L15" s="97">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="31">
+        <v>3</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="48">
+        <v>10</v>
+      </c>
+      <c r="I16" s="38">
+        <v>64</v>
+      </c>
+      <c r="J16" s="38"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="99">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="31">
+        <v>3</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="48">
+        <v>50</v>
+      </c>
+      <c r="I17" s="38">
+        <v>64</v>
+      </c>
+      <c r="J17" s="38"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="99">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
+        <v>3</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="48">
+        <v>100</v>
+      </c>
+      <c r="I18" s="38">
+        <v>64</v>
+      </c>
+      <c r="J18" s="38"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="99">
+        <v>13</v>
+      </c>
       <c r="P18" t="s">
         <v>85</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="31">
+        <v>3</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="48">
+        <v>150</v>
+      </c>
+      <c r="I19" s="38">
+        <v>64</v>
+      </c>
+      <c r="J19" s="38">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="K19" s="33">
+        <v>0.151</v>
+      </c>
+      <c r="L19" s="99">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
+        <v>3</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="48">
+        <v>200</v>
+      </c>
+      <c r="I20" s="38">
+        <v>64</v>
+      </c>
+      <c r="J20" s="38">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="K20" s="33">
+        <v>0.157</v>
+      </c>
+      <c r="L20" s="99">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="31">
+        <v>3</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="48">
+        <v>250</v>
+      </c>
+      <c r="I21" s="38">
+        <v>64</v>
+      </c>
+      <c r="J21" s="38">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="K21" s="33">
+        <v>0.125</v>
+      </c>
+      <c r="L21" s="99">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="31">
+        <v>3</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="48">
+        <v>300</v>
+      </c>
+      <c r="I22" s="38">
+        <v>64</v>
+      </c>
+      <c r="J22" s="38">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="K22" s="33">
+        <v>0.182</v>
+      </c>
+      <c r="L22" s="99">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="31">
+        <v>3</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="48">
+        <v>350</v>
+      </c>
+      <c r="I23" s="38">
+        <v>64</v>
+      </c>
+      <c r="J23" s="38">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="K23" s="33">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L23" s="99">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="31">
+        <v>3</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="48">
+        <v>400</v>
+      </c>
+      <c r="I24" s="38">
+        <v>64</v>
+      </c>
+      <c r="J24" s="38">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="K24" s="33">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="L24" s="99">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="31">
+        <v>3</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="48">
+        <v>450</v>
+      </c>
+      <c r="I25" s="38">
+        <v>64</v>
+      </c>
+      <c r="J25" s="38">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="K25" s="33">
+        <v>0.121</v>
+      </c>
+      <c r="L25" s="99">
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="16:16" x14ac:dyDescent="0.25">
@@ -14266,6 +15872,62 @@
     <row r="68" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P68" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="93" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="P93" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA93" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="P118" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA118" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="144" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="P144" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA144" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="170" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="P170" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA170" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="196" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="P196" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA196" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="221" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="P221" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA221" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="246" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="P246" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA246" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating NN analysis results
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B880416-3E48-445B-A786-64855C79913C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995E31FF-EDAC-4849-B792-300F491A3302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
@@ -7027,6 +7027,128 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C542260-C6D2-46F8-0C10-853A31A220EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="44662725" y="35937825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF03C233-E2A7-074D-6AF8-96269B87CB6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="44662725" y="40890825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -17043,8 +17165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546EE643-96AE-406E-920D-B005CB201B4A}">
   <dimension ref="B3:DI291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="C38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19618,8 +19740,12 @@
       <c r="J52" s="38">
         <v>32</v>
       </c>
-      <c r="K52" s="38"/>
-      <c r="L52" s="33"/>
+      <c r="K52" s="38">
+        <v>0.97</v>
+      </c>
+      <c r="L52" s="33">
+        <v>0.108</v>
+      </c>
       <c r="M52" s="99">
         <v>47</v>
       </c>
@@ -19666,8 +19792,12 @@
       <c r="J53" s="38">
         <v>32</v>
       </c>
-      <c r="K53" s="38"/>
-      <c r="L53" s="33"/>
+      <c r="K53" s="38">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="L53" s="33">
+        <v>0.111</v>
+      </c>
       <c r="M53" s="99">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Updating neural network run results looking at batch sizes and learning rates
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995E31FF-EDAC-4849-B792-300F491A3302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACF5C44-9961-47EA-81B4-6CBFAC1BC207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
@@ -1135,7 +1135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1535,6 +1535,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7149,6 +7152,738 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{363555AA-A65B-3792-E6B0-955838A15972}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="44662725" y="45653325"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD8FAF72-6579-B1DB-25CF-4BD0A01B9951}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="44662725" y="50415825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>89</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CE91091-382D-BB73-377D-C6D99D7BEC1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="6934200"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBB0E0D8-7039-1604-0187-31F8E5EB0D33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="11715750"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB3B8239-170B-D59C-FB00-9B202EF7705B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="16506825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8B6B19E-4362-3A86-D289-C85BD2FF7FE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="21269325"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BD886C3-F04A-56F6-B445-09283D867A4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="26031825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{121441E9-4C4B-E6EA-21B3-27D31141B260}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="30984825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4845BF91-3593-F907-253F-04FD5D782788}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="35937825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CDB9E53-DF15-EEE7-9ABA-428F23FE7166}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="40890825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F25C726-9A65-C5BB-157D-90309302337C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId62">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="45653325"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55CFEBE6-06DA-9DC5-D897-10F86894A7A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId63">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="51368325" y="50415825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -17165,8 +17900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546EE643-96AE-406E-920D-B005CB201B4A}">
   <dimension ref="B3:DI291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19844,8 +20579,12 @@
       <c r="J54" s="38">
         <v>32</v>
       </c>
-      <c r="K54" s="38"/>
-      <c r="L54" s="33"/>
+      <c r="K54" s="38">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="L54" s="33">
+        <v>0.126</v>
+      </c>
       <c r="M54" s="99">
         <v>49</v>
       </c>
@@ -19892,8 +20631,12 @@
       <c r="J55" s="42">
         <v>32</v>
       </c>
-      <c r="K55" s="42"/>
-      <c r="L55" s="4"/>
+      <c r="K55" s="42">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="L55" s="4">
+        <v>8.5999999999999993E-2</v>
+      </c>
       <c r="M55" s="97">
         <v>50</v>
       </c>
@@ -19940,8 +20683,12 @@
       <c r="J56" s="114">
         <v>64</v>
       </c>
-      <c r="K56" s="114"/>
-      <c r="L56" s="115"/>
+      <c r="K56" s="114">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="L56" s="115">
+        <v>0.95599999999999996</v>
+      </c>
       <c r="M56" s="119">
         <v>51</v>
       </c>
@@ -19988,8 +20735,12 @@
       <c r="J57" s="38">
         <v>64</v>
       </c>
-      <c r="K57" s="38"/>
-      <c r="L57" s="33"/>
+      <c r="K57" s="38">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="L57" s="33">
+        <v>0.35799999999999998</v>
+      </c>
       <c r="M57" s="99">
         <v>52</v>
       </c>
@@ -20036,9 +20787,13 @@
       <c r="J58" s="38">
         <v>64</v>
       </c>
-      <c r="K58" s="38"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="99">
+      <c r="K58" s="38">
+        <v>0.95</v>
+      </c>
+      <c r="L58" s="33">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="M58" s="141">
         <v>53</v>
       </c>
       <c r="Q58" s="106"/>
@@ -20084,8 +20839,12 @@
       <c r="J59" s="38">
         <v>64</v>
       </c>
-      <c r="K59" s="38"/>
-      <c r="L59" s="33"/>
+      <c r="K59" s="38">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="L59" s="33">
+        <v>0.16400000000000001</v>
+      </c>
       <c r="M59" s="99">
         <v>54</v>
       </c>
@@ -20132,8 +20891,12 @@
       <c r="J60" s="38">
         <v>64</v>
       </c>
-      <c r="K60" s="38"/>
-      <c r="L60" s="33"/>
+      <c r="K60" s="38">
+        <v>0.96</v>
+      </c>
+      <c r="L60" s="33">
+        <v>0.154</v>
+      </c>
       <c r="M60" s="99">
         <v>55</v>
       </c>
@@ -20180,9 +20943,13 @@
       <c r="J61" s="38">
         <v>64</v>
       </c>
-      <c r="K61" s="38"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="99">
+      <c r="K61" s="38">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="L61" s="33">
+        <v>0.122</v>
+      </c>
+      <c r="M61" s="141">
         <v>56</v>
       </c>
       <c r="Q61" s="106"/>
@@ -20252,9 +21019,13 @@
       <c r="J62" s="38">
         <v>64</v>
       </c>
-      <c r="K62" s="38"/>
-      <c r="L62" s="33"/>
-      <c r="M62" s="99">
+      <c r="K62" s="38">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="L62" s="33">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="M62" s="141">
         <v>57</v>
       </c>
       <c r="Q62" s="106"/>
@@ -20300,8 +21071,12 @@
       <c r="J63" s="38">
         <v>64</v>
       </c>
-      <c r="K63" s="38"/>
-      <c r="L63" s="33"/>
+      <c r="K63" s="38">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="L63" s="33">
+        <v>0.127</v>
+      </c>
       <c r="M63" s="99">
         <v>58</v>
       </c>
@@ -20348,8 +21123,12 @@
       <c r="J64" s="38">
         <v>64</v>
       </c>
-      <c r="K64" s="38"/>
-      <c r="L64" s="33"/>
+      <c r="K64" s="38">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="L64" s="33">
+        <v>0.158</v>
+      </c>
       <c r="M64" s="99">
         <v>59</v>
       </c>
@@ -20396,8 +21175,12 @@
       <c r="J65" s="42">
         <v>64</v>
       </c>
-      <c r="K65" s="42"/>
-      <c r="L65" s="4"/>
+      <c r="K65" s="42">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="L65" s="4">
+        <v>0.17199999999999999</v>
+      </c>
       <c r="M65" s="97">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Updating NN analysis work
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACF5C44-9961-47EA-81B4-6CBFAC1BC207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1FF35C-7887-40D6-8199-D3E717B5F1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="123">
   <si>
     <t xml:space="preserve">Model: </t>
   </si>
@@ -381,6 +381,36 @@
   <si>
     <t>#60</t>
   </si>
+  <si>
+    <t>#61</t>
+  </si>
+  <si>
+    <t>#62</t>
+  </si>
+  <si>
+    <t>#63</t>
+  </si>
+  <si>
+    <t>#64</t>
+  </si>
+  <si>
+    <t>#65</t>
+  </si>
+  <si>
+    <t>#66</t>
+  </si>
+  <si>
+    <t>#67</t>
+  </si>
+  <si>
+    <t>#68</t>
+  </si>
+  <si>
+    <t>#69</t>
+  </si>
+  <si>
+    <t>#70</t>
+  </si>
 </sst>
 </file>
 
@@ -410,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +474,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1135,7 +1171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1486,6 +1522,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1537,7 +1576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7884,6 +7923,555 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>99</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B44C2A3C-A971-9D44-4A99-22C5C32D2039}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId64">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="58073925" y="6934200"/>
+          <a:ext cx="5476875" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>99</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38118ACB-A60A-EA57-2FCC-C9EB46EB8F67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId65">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="58073925" y="11715750"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>99</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A743BA9-ACEA-BB88-A379-10FDA9491142}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="58073925" y="16506825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>99</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23758745-1E49-6FBA-398F-EB7677E8EA50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId67">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="58073925" y="21459825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>99</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Picture 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0B78B45-6702-712D-7048-46AD23D06A3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId68">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="58073925" y="26222325"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>100</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7FB743F-E9F2-DED5-46B4-87FAC06E63A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId69">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="58073925" y="31175325"/>
+          <a:ext cx="5486400" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>99</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Picture 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61FAA7A6-867C-2D85-8469-4C5AED611F7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId70">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="58073925" y="35937825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>99</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Picture 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{626DDE06-87F1-D4ED-B878-90610301F4DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId71">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="58073925" y="40890825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>91</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>99</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Picture 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A52A6B5-42F2-A8ED-1FDD-4678E29BFA1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId72">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="58073925" y="45843825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8293,22 +8881,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="124" t="s">
+      <c r="B5" s="126"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="125" t="s">
+      <c r="E5" s="126"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -9713,22 +10301,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="124" t="s">
+      <c r="B5" s="126"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="125" t="s">
+      <c r="E5" s="126"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -11133,22 +11721,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="124" t="s">
+      <c r="B5" s="126"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="125" t="s">
+      <c r="E5" s="126"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -12553,22 +13141,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="124" t="s">
+      <c r="B5" s="126"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="125" t="s">
+      <c r="E5" s="126"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -13973,22 +14561,22 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="124" t="s">
+      <c r="B5" s="126"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="125" t="s">
+      <c r="E5" s="126"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -15373,22 +15961,22 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="124" t="s">
+      <c r="B5" s="126"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="125" t="s">
+      <c r="E5" s="126"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125"/>
-      <c r="J5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
       <c r="K5" s="95"/>
       <c r="L5" s="108"/>
       <c r="M5" s="108"/>
@@ -17900,8 +18488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546EE643-96AE-406E-920D-B005CB201B4A}">
   <dimension ref="B3:DI291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L66" sqref="L66"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17919,25 +18507,25 @@
   <sheetData>
     <row r="3" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="127"/>
       <c r="E4" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="124" t="s">
+      <c r="F4" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="125"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="125" t="s">
+      <c r="G4" s="126"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="127"/>
       <c r="M4" s="95"/>
       <c r="N4" s="123"/>
       <c r="O4" s="122" t="s">
@@ -19028,102 +19616,102 @@
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="Q31" s="127" t="s">
+      <c r="Q31" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="R31" s="128"/>
-      <c r="S31" s="128"/>
-      <c r="T31" s="128"/>
-      <c r="U31" s="128"/>
-      <c r="V31" s="128"/>
-      <c r="W31" s="128"/>
-      <c r="X31" s="128"/>
-      <c r="Y31" s="128"/>
-      <c r="Z31" s="128"/>
-      <c r="AA31" s="128"/>
-      <c r="AB31" s="128"/>
-      <c r="AC31" s="128"/>
-      <c r="AD31" s="128"/>
-      <c r="AE31" s="128"/>
-      <c r="AF31" s="128"/>
-      <c r="AG31" s="128"/>
-      <c r="AH31" s="128"/>
-      <c r="AI31" s="128"/>
-      <c r="AJ31" s="128"/>
-      <c r="AK31" s="128"/>
-      <c r="AL31" s="128"/>
-      <c r="AM31" s="128"/>
-      <c r="AN31" s="128"/>
-      <c r="AO31" s="128"/>
-      <c r="AP31" s="128"/>
-      <c r="AQ31" s="128"/>
-      <c r="AR31" s="128"/>
-      <c r="AS31" s="128"/>
-      <c r="AT31" s="128"/>
-      <c r="AU31" s="128"/>
-      <c r="AV31" s="128"/>
-      <c r="AW31" s="128"/>
-      <c r="AX31" s="128"/>
-      <c r="AY31" s="128"/>
-      <c r="AZ31" s="128"/>
-      <c r="BA31" s="128"/>
-      <c r="BB31" s="128"/>
-      <c r="BC31" s="128"/>
-      <c r="BD31" s="128"/>
-      <c r="BE31" s="128"/>
-      <c r="BF31" s="128"/>
-      <c r="BG31" s="128"/>
-      <c r="BH31" s="128"/>
-      <c r="BI31" s="128"/>
-      <c r="BJ31" s="129"/>
-      <c r="BP31" s="127" t="s">
+      <c r="R31" s="129"/>
+      <c r="S31" s="129"/>
+      <c r="T31" s="129"/>
+      <c r="U31" s="129"/>
+      <c r="V31" s="129"/>
+      <c r="W31" s="129"/>
+      <c r="X31" s="129"/>
+      <c r="Y31" s="129"/>
+      <c r="Z31" s="129"/>
+      <c r="AA31" s="129"/>
+      <c r="AB31" s="129"/>
+      <c r="AC31" s="129"/>
+      <c r="AD31" s="129"/>
+      <c r="AE31" s="129"/>
+      <c r="AF31" s="129"/>
+      <c r="AG31" s="129"/>
+      <c r="AH31" s="129"/>
+      <c r="AI31" s="129"/>
+      <c r="AJ31" s="129"/>
+      <c r="AK31" s="129"/>
+      <c r="AL31" s="129"/>
+      <c r="AM31" s="129"/>
+      <c r="AN31" s="129"/>
+      <c r="AO31" s="129"/>
+      <c r="AP31" s="129"/>
+      <c r="AQ31" s="129"/>
+      <c r="AR31" s="129"/>
+      <c r="AS31" s="129"/>
+      <c r="AT31" s="129"/>
+      <c r="AU31" s="129"/>
+      <c r="AV31" s="129"/>
+      <c r="AW31" s="129"/>
+      <c r="AX31" s="129"/>
+      <c r="AY31" s="129"/>
+      <c r="AZ31" s="129"/>
+      <c r="BA31" s="129"/>
+      <c r="BB31" s="129"/>
+      <c r="BC31" s="129"/>
+      <c r="BD31" s="129"/>
+      <c r="BE31" s="129"/>
+      <c r="BF31" s="129"/>
+      <c r="BG31" s="129"/>
+      <c r="BH31" s="129"/>
+      <c r="BI31" s="129"/>
+      <c r="BJ31" s="130"/>
+      <c r="BP31" s="128" t="s">
         <v>92</v>
       </c>
-      <c r="BQ31" s="128"/>
-      <c r="BR31" s="128"/>
-      <c r="BS31" s="128"/>
-      <c r="BT31" s="128"/>
-      <c r="BU31" s="128"/>
-      <c r="BV31" s="128"/>
-      <c r="BW31" s="128"/>
-      <c r="BX31" s="128"/>
-      <c r="BY31" s="128"/>
-      <c r="BZ31" s="128"/>
-      <c r="CA31" s="128"/>
-      <c r="CB31" s="128"/>
-      <c r="CC31" s="128"/>
-      <c r="CD31" s="128"/>
-      <c r="CE31" s="128"/>
-      <c r="CF31" s="128"/>
-      <c r="CG31" s="128"/>
-      <c r="CH31" s="128"/>
-      <c r="CI31" s="128"/>
-      <c r="CJ31" s="128"/>
-      <c r="CK31" s="128"/>
-      <c r="CL31" s="128"/>
-      <c r="CM31" s="128"/>
-      <c r="CN31" s="128"/>
-      <c r="CO31" s="128"/>
-      <c r="CP31" s="128"/>
-      <c r="CQ31" s="128"/>
-      <c r="CR31" s="128"/>
-      <c r="CS31" s="128"/>
-      <c r="CT31" s="128"/>
-      <c r="CU31" s="128"/>
-      <c r="CV31" s="128"/>
-      <c r="CW31" s="128"/>
-      <c r="CX31" s="128"/>
-      <c r="CY31" s="128"/>
-      <c r="CZ31" s="128"/>
-      <c r="DA31" s="128"/>
-      <c r="DB31" s="128"/>
-      <c r="DC31" s="128"/>
-      <c r="DD31" s="128"/>
-      <c r="DE31" s="128"/>
-      <c r="DF31" s="128"/>
-      <c r="DG31" s="128"/>
-      <c r="DH31" s="128"/>
-      <c r="DI31" s="129"/>
+      <c r="BQ31" s="129"/>
+      <c r="BR31" s="129"/>
+      <c r="BS31" s="129"/>
+      <c r="BT31" s="129"/>
+      <c r="BU31" s="129"/>
+      <c r="BV31" s="129"/>
+      <c r="BW31" s="129"/>
+      <c r="BX31" s="129"/>
+      <c r="BY31" s="129"/>
+      <c r="BZ31" s="129"/>
+      <c r="CA31" s="129"/>
+      <c r="CB31" s="129"/>
+      <c r="CC31" s="129"/>
+      <c r="CD31" s="129"/>
+      <c r="CE31" s="129"/>
+      <c r="CF31" s="129"/>
+      <c r="CG31" s="129"/>
+      <c r="CH31" s="129"/>
+      <c r="CI31" s="129"/>
+      <c r="CJ31" s="129"/>
+      <c r="CK31" s="129"/>
+      <c r="CL31" s="129"/>
+      <c r="CM31" s="129"/>
+      <c r="CN31" s="129"/>
+      <c r="CO31" s="129"/>
+      <c r="CP31" s="129"/>
+      <c r="CQ31" s="129"/>
+      <c r="CR31" s="129"/>
+      <c r="CS31" s="129"/>
+      <c r="CT31" s="129"/>
+      <c r="CU31" s="129"/>
+      <c r="CV31" s="129"/>
+      <c r="CW31" s="129"/>
+      <c r="CX31" s="129"/>
+      <c r="CY31" s="129"/>
+      <c r="CZ31" s="129"/>
+      <c r="DA31" s="129"/>
+      <c r="DB31" s="129"/>
+      <c r="DC31" s="129"/>
+      <c r="DD31" s="129"/>
+      <c r="DE31" s="129"/>
+      <c r="DF31" s="129"/>
+      <c r="DG31" s="129"/>
+      <c r="DH31" s="129"/>
+      <c r="DI31" s="130"/>
     </row>
     <row r="32" spans="2:113" x14ac:dyDescent="0.25">
       <c r="B32" s="31">
@@ -19164,98 +19752,98 @@
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="Q32" s="130"/>
-      <c r="R32" s="131"/>
-      <c r="S32" s="131"/>
-      <c r="T32" s="131"/>
-      <c r="U32" s="131"/>
-      <c r="V32" s="131"/>
-      <c r="W32" s="131"/>
-      <c r="X32" s="131"/>
-      <c r="Y32" s="131"/>
-      <c r="Z32" s="131"/>
-      <c r="AA32" s="131"/>
-      <c r="AB32" s="131"/>
-      <c r="AC32" s="131"/>
-      <c r="AD32" s="131"/>
-      <c r="AE32" s="131"/>
-      <c r="AF32" s="131"/>
-      <c r="AG32" s="131"/>
-      <c r="AH32" s="131"/>
-      <c r="AI32" s="131"/>
-      <c r="AJ32" s="131"/>
-      <c r="AK32" s="131"/>
-      <c r="AL32" s="131"/>
-      <c r="AM32" s="131"/>
-      <c r="AN32" s="131"/>
-      <c r="AO32" s="131"/>
-      <c r="AP32" s="131"/>
-      <c r="AQ32" s="131"/>
-      <c r="AR32" s="131"/>
-      <c r="AS32" s="131"/>
-      <c r="AT32" s="131"/>
-      <c r="AU32" s="131"/>
-      <c r="AV32" s="131"/>
-      <c r="AW32" s="131"/>
-      <c r="AX32" s="131"/>
-      <c r="AY32" s="131"/>
-      <c r="AZ32" s="131"/>
-      <c r="BA32" s="131"/>
-      <c r="BB32" s="131"/>
-      <c r="BC32" s="131"/>
-      <c r="BD32" s="131"/>
-      <c r="BE32" s="131"/>
-      <c r="BF32" s="131"/>
-      <c r="BG32" s="131"/>
-      <c r="BH32" s="131"/>
-      <c r="BI32" s="131"/>
-      <c r="BJ32" s="132"/>
-      <c r="BP32" s="130"/>
-      <c r="BQ32" s="131"/>
-      <c r="BR32" s="131"/>
-      <c r="BS32" s="131"/>
-      <c r="BT32" s="131"/>
-      <c r="BU32" s="131"/>
-      <c r="BV32" s="131"/>
-      <c r="BW32" s="131"/>
-      <c r="BX32" s="131"/>
-      <c r="BY32" s="131"/>
-      <c r="BZ32" s="131"/>
-      <c r="CA32" s="131"/>
-      <c r="CB32" s="131"/>
-      <c r="CC32" s="131"/>
-      <c r="CD32" s="131"/>
-      <c r="CE32" s="131"/>
-      <c r="CF32" s="131"/>
-      <c r="CG32" s="131"/>
-      <c r="CH32" s="131"/>
-      <c r="CI32" s="131"/>
-      <c r="CJ32" s="131"/>
-      <c r="CK32" s="131"/>
-      <c r="CL32" s="131"/>
-      <c r="CM32" s="131"/>
-      <c r="CN32" s="131"/>
-      <c r="CO32" s="131"/>
-      <c r="CP32" s="131"/>
-      <c r="CQ32" s="131"/>
-      <c r="CR32" s="131"/>
-      <c r="CS32" s="131"/>
-      <c r="CT32" s="131"/>
-      <c r="CU32" s="131"/>
-      <c r="CV32" s="131"/>
-      <c r="CW32" s="131"/>
-      <c r="CX32" s="131"/>
-      <c r="CY32" s="131"/>
-      <c r="CZ32" s="131"/>
-      <c r="DA32" s="131"/>
-      <c r="DB32" s="131"/>
-      <c r="DC32" s="131"/>
-      <c r="DD32" s="131"/>
-      <c r="DE32" s="131"/>
-      <c r="DF32" s="131"/>
-      <c r="DG32" s="131"/>
-      <c r="DH32" s="131"/>
-      <c r="DI32" s="132"/>
+      <c r="Q32" s="131"/>
+      <c r="R32" s="132"/>
+      <c r="S32" s="132"/>
+      <c r="T32" s="132"/>
+      <c r="U32" s="132"/>
+      <c r="V32" s="132"/>
+      <c r="W32" s="132"/>
+      <c r="X32" s="132"/>
+      <c r="Y32" s="132"/>
+      <c r="Z32" s="132"/>
+      <c r="AA32" s="132"/>
+      <c r="AB32" s="132"/>
+      <c r="AC32" s="132"/>
+      <c r="AD32" s="132"/>
+      <c r="AE32" s="132"/>
+      <c r="AF32" s="132"/>
+      <c r="AG32" s="132"/>
+      <c r="AH32" s="132"/>
+      <c r="AI32" s="132"/>
+      <c r="AJ32" s="132"/>
+      <c r="AK32" s="132"/>
+      <c r="AL32" s="132"/>
+      <c r="AM32" s="132"/>
+      <c r="AN32" s="132"/>
+      <c r="AO32" s="132"/>
+      <c r="AP32" s="132"/>
+      <c r="AQ32" s="132"/>
+      <c r="AR32" s="132"/>
+      <c r="AS32" s="132"/>
+      <c r="AT32" s="132"/>
+      <c r="AU32" s="132"/>
+      <c r="AV32" s="132"/>
+      <c r="AW32" s="132"/>
+      <c r="AX32" s="132"/>
+      <c r="AY32" s="132"/>
+      <c r="AZ32" s="132"/>
+      <c r="BA32" s="132"/>
+      <c r="BB32" s="132"/>
+      <c r="BC32" s="132"/>
+      <c r="BD32" s="132"/>
+      <c r="BE32" s="132"/>
+      <c r="BF32" s="132"/>
+      <c r="BG32" s="132"/>
+      <c r="BH32" s="132"/>
+      <c r="BI32" s="132"/>
+      <c r="BJ32" s="133"/>
+      <c r="BP32" s="131"/>
+      <c r="BQ32" s="132"/>
+      <c r="BR32" s="132"/>
+      <c r="BS32" s="132"/>
+      <c r="BT32" s="132"/>
+      <c r="BU32" s="132"/>
+      <c r="BV32" s="132"/>
+      <c r="BW32" s="132"/>
+      <c r="BX32" s="132"/>
+      <c r="BY32" s="132"/>
+      <c r="BZ32" s="132"/>
+      <c r="CA32" s="132"/>
+      <c r="CB32" s="132"/>
+      <c r="CC32" s="132"/>
+      <c r="CD32" s="132"/>
+      <c r="CE32" s="132"/>
+      <c r="CF32" s="132"/>
+      <c r="CG32" s="132"/>
+      <c r="CH32" s="132"/>
+      <c r="CI32" s="132"/>
+      <c r="CJ32" s="132"/>
+      <c r="CK32" s="132"/>
+      <c r="CL32" s="132"/>
+      <c r="CM32" s="132"/>
+      <c r="CN32" s="132"/>
+      <c r="CO32" s="132"/>
+      <c r="CP32" s="132"/>
+      <c r="CQ32" s="132"/>
+      <c r="CR32" s="132"/>
+      <c r="CS32" s="132"/>
+      <c r="CT32" s="132"/>
+      <c r="CU32" s="132"/>
+      <c r="CV32" s="132"/>
+      <c r="CW32" s="132"/>
+      <c r="CX32" s="132"/>
+      <c r="CY32" s="132"/>
+      <c r="CZ32" s="132"/>
+      <c r="DA32" s="132"/>
+      <c r="DB32" s="132"/>
+      <c r="DC32" s="132"/>
+      <c r="DD32" s="132"/>
+      <c r="DE32" s="132"/>
+      <c r="DF32" s="132"/>
+      <c r="DG32" s="132"/>
+      <c r="DH32" s="132"/>
+      <c r="DI32" s="133"/>
     </row>
     <row r="33" spans="2:113" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="31">
@@ -19296,98 +19884,98 @@
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="Q33" s="133"/>
-      <c r="R33" s="134"/>
-      <c r="S33" s="134"/>
-      <c r="T33" s="134"/>
-      <c r="U33" s="134"/>
-      <c r="V33" s="134"/>
-      <c r="W33" s="134"/>
-      <c r="X33" s="134"/>
-      <c r="Y33" s="134"/>
-      <c r="Z33" s="134"/>
-      <c r="AA33" s="134"/>
-      <c r="AB33" s="134"/>
-      <c r="AC33" s="134"/>
-      <c r="AD33" s="134"/>
-      <c r="AE33" s="134"/>
-      <c r="AF33" s="134"/>
-      <c r="AG33" s="134"/>
-      <c r="AH33" s="134"/>
-      <c r="AI33" s="134"/>
-      <c r="AJ33" s="134"/>
-      <c r="AK33" s="134"/>
-      <c r="AL33" s="134"/>
-      <c r="AM33" s="134"/>
-      <c r="AN33" s="134"/>
-      <c r="AO33" s="134"/>
-      <c r="AP33" s="134"/>
-      <c r="AQ33" s="134"/>
-      <c r="AR33" s="134"/>
-      <c r="AS33" s="134"/>
-      <c r="AT33" s="134"/>
-      <c r="AU33" s="134"/>
-      <c r="AV33" s="134"/>
-      <c r="AW33" s="134"/>
-      <c r="AX33" s="134"/>
-      <c r="AY33" s="134"/>
-      <c r="AZ33" s="134"/>
-      <c r="BA33" s="134"/>
-      <c r="BB33" s="134"/>
-      <c r="BC33" s="134"/>
-      <c r="BD33" s="134"/>
-      <c r="BE33" s="134"/>
-      <c r="BF33" s="134"/>
-      <c r="BG33" s="134"/>
-      <c r="BH33" s="134"/>
-      <c r="BI33" s="134"/>
-      <c r="BJ33" s="135"/>
-      <c r="BP33" s="133"/>
-      <c r="BQ33" s="134"/>
-      <c r="BR33" s="134"/>
-      <c r="BS33" s="134"/>
-      <c r="BT33" s="134"/>
-      <c r="BU33" s="134"/>
-      <c r="BV33" s="134"/>
-      <c r="BW33" s="134"/>
-      <c r="BX33" s="134"/>
-      <c r="BY33" s="134"/>
-      <c r="BZ33" s="134"/>
-      <c r="CA33" s="134"/>
-      <c r="CB33" s="134"/>
-      <c r="CC33" s="134"/>
-      <c r="CD33" s="134"/>
-      <c r="CE33" s="134"/>
-      <c r="CF33" s="134"/>
-      <c r="CG33" s="134"/>
-      <c r="CH33" s="134"/>
-      <c r="CI33" s="134"/>
-      <c r="CJ33" s="134"/>
-      <c r="CK33" s="134"/>
-      <c r="CL33" s="134"/>
-      <c r="CM33" s="134"/>
-      <c r="CN33" s="134"/>
-      <c r="CO33" s="134"/>
-      <c r="CP33" s="134"/>
-      <c r="CQ33" s="134"/>
-      <c r="CR33" s="134"/>
-      <c r="CS33" s="134"/>
-      <c r="CT33" s="134"/>
-      <c r="CU33" s="134"/>
-      <c r="CV33" s="134"/>
-      <c r="CW33" s="134"/>
-      <c r="CX33" s="134"/>
-      <c r="CY33" s="134"/>
-      <c r="CZ33" s="134"/>
-      <c r="DA33" s="134"/>
-      <c r="DB33" s="134"/>
-      <c r="DC33" s="134"/>
-      <c r="DD33" s="134"/>
-      <c r="DE33" s="134"/>
-      <c r="DF33" s="134"/>
-      <c r="DG33" s="134"/>
-      <c r="DH33" s="134"/>
-      <c r="DI33" s="135"/>
+      <c r="Q33" s="134"/>
+      <c r="R33" s="135"/>
+      <c r="S33" s="135"/>
+      <c r="T33" s="135"/>
+      <c r="U33" s="135"/>
+      <c r="V33" s="135"/>
+      <c r="W33" s="135"/>
+      <c r="X33" s="135"/>
+      <c r="Y33" s="135"/>
+      <c r="Z33" s="135"/>
+      <c r="AA33" s="135"/>
+      <c r="AB33" s="135"/>
+      <c r="AC33" s="135"/>
+      <c r="AD33" s="135"/>
+      <c r="AE33" s="135"/>
+      <c r="AF33" s="135"/>
+      <c r="AG33" s="135"/>
+      <c r="AH33" s="135"/>
+      <c r="AI33" s="135"/>
+      <c r="AJ33" s="135"/>
+      <c r="AK33" s="135"/>
+      <c r="AL33" s="135"/>
+      <c r="AM33" s="135"/>
+      <c r="AN33" s="135"/>
+      <c r="AO33" s="135"/>
+      <c r="AP33" s="135"/>
+      <c r="AQ33" s="135"/>
+      <c r="AR33" s="135"/>
+      <c r="AS33" s="135"/>
+      <c r="AT33" s="135"/>
+      <c r="AU33" s="135"/>
+      <c r="AV33" s="135"/>
+      <c r="AW33" s="135"/>
+      <c r="AX33" s="135"/>
+      <c r="AY33" s="135"/>
+      <c r="AZ33" s="135"/>
+      <c r="BA33" s="135"/>
+      <c r="BB33" s="135"/>
+      <c r="BC33" s="135"/>
+      <c r="BD33" s="135"/>
+      <c r="BE33" s="135"/>
+      <c r="BF33" s="135"/>
+      <c r="BG33" s="135"/>
+      <c r="BH33" s="135"/>
+      <c r="BI33" s="135"/>
+      <c r="BJ33" s="136"/>
+      <c r="BP33" s="134"/>
+      <c r="BQ33" s="135"/>
+      <c r="BR33" s="135"/>
+      <c r="BS33" s="135"/>
+      <c r="BT33" s="135"/>
+      <c r="BU33" s="135"/>
+      <c r="BV33" s="135"/>
+      <c r="BW33" s="135"/>
+      <c r="BX33" s="135"/>
+      <c r="BY33" s="135"/>
+      <c r="BZ33" s="135"/>
+      <c r="CA33" s="135"/>
+      <c r="CB33" s="135"/>
+      <c r="CC33" s="135"/>
+      <c r="CD33" s="135"/>
+      <c r="CE33" s="135"/>
+      <c r="CF33" s="135"/>
+      <c r="CG33" s="135"/>
+      <c r="CH33" s="135"/>
+      <c r="CI33" s="135"/>
+      <c r="CJ33" s="135"/>
+      <c r="CK33" s="135"/>
+      <c r="CL33" s="135"/>
+      <c r="CM33" s="135"/>
+      <c r="CN33" s="135"/>
+      <c r="CO33" s="135"/>
+      <c r="CP33" s="135"/>
+      <c r="CQ33" s="135"/>
+      <c r="CR33" s="135"/>
+      <c r="CS33" s="135"/>
+      <c r="CT33" s="135"/>
+      <c r="CU33" s="135"/>
+      <c r="CV33" s="135"/>
+      <c r="CW33" s="135"/>
+      <c r="CX33" s="135"/>
+      <c r="CY33" s="135"/>
+      <c r="CZ33" s="135"/>
+      <c r="DA33" s="135"/>
+      <c r="DB33" s="135"/>
+      <c r="DC33" s="135"/>
+      <c r="DD33" s="135"/>
+      <c r="DE33" s="135"/>
+      <c r="DF33" s="135"/>
+      <c r="DG33" s="135"/>
+      <c r="DH33" s="135"/>
+      <c r="DI33" s="136"/>
     </row>
     <row r="34" spans="2:113" x14ac:dyDescent="0.25">
       <c r="B34" s="31">
@@ -19644,7 +20232,7 @@
       </c>
       <c r="CL36" s="102"/>
       <c r="CN36" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="CX36" s="102"/>
       <c r="CY36" s="106"/>
@@ -20793,7 +21381,7 @@
       <c r="L58" s="33">
         <v>0.17899999999999999</v>
       </c>
-      <c r="M58" s="141">
+      <c r="M58" s="124">
         <v>53</v>
       </c>
       <c r="Q58" s="106"/>
@@ -20949,7 +21537,7 @@
       <c r="L61" s="33">
         <v>0.122</v>
       </c>
-      <c r="M61" s="141">
+      <c r="M61" s="124">
         <v>56</v>
       </c>
       <c r="Q61" s="106"/>
@@ -20982,7 +21570,7 @@
       </c>
       <c r="CL61" s="102"/>
       <c r="CN61" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="CX61" s="102"/>
       <c r="CY61" s="106"/>
@@ -21025,7 +21613,7 @@
       <c r="L62" s="33">
         <v>0.13900000000000001</v>
       </c>
-      <c r="M62" s="141">
+      <c r="M62" s="124">
         <v>57</v>
       </c>
       <c r="Q62" s="106"/>
@@ -21227,8 +21815,12 @@
       <c r="J66" s="38">
         <v>128</v>
       </c>
-      <c r="K66" s="38"/>
-      <c r="L66" s="33"/>
+      <c r="K66" s="38">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="L66" s="33">
+        <v>1.5449999999999999</v>
+      </c>
       <c r="M66" s="119">
         <v>61</v>
       </c>
@@ -21275,8 +21867,12 @@
       <c r="J67" s="38">
         <v>128</v>
       </c>
-      <c r="K67" s="38"/>
-      <c r="L67" s="33"/>
+      <c r="K67" s="38">
+        <v>0.751</v>
+      </c>
+      <c r="L67" s="33">
+        <v>0.58799999999999997</v>
+      </c>
       <c r="M67" s="99">
         <v>62</v>
       </c>
@@ -21323,9 +21919,13 @@
       <c r="J68" s="38">
         <v>128</v>
       </c>
-      <c r="K68" s="38"/>
-      <c r="L68" s="33"/>
-      <c r="M68" s="99">
+      <c r="K68" s="38">
+        <v>0.92</v>
+      </c>
+      <c r="L68" s="33">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="M68" s="142">
         <v>63</v>
       </c>
       <c r="Q68" s="106"/>
@@ -21371,8 +21971,12 @@
       <c r="J69" s="38">
         <v>128</v>
       </c>
-      <c r="K69" s="38"/>
-      <c r="L69" s="33"/>
+      <c r="K69" s="38">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="L69" s="33">
+        <v>0.32400000000000001</v>
+      </c>
       <c r="M69" s="99">
         <v>64</v>
       </c>
@@ -21419,9 +22023,13 @@
       <c r="J70" s="38">
         <v>128</v>
       </c>
-      <c r="K70" s="38"/>
-      <c r="L70" s="33"/>
-      <c r="M70" s="99">
+      <c r="K70" s="38">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="L70" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="M70" s="142">
         <v>65</v>
       </c>
       <c r="Q70" s="106"/>
@@ -21467,8 +22075,12 @@
       <c r="J71" s="38">
         <v>128</v>
       </c>
-      <c r="K71" s="38"/>
-      <c r="L71" s="33"/>
+      <c r="K71" s="38">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="L71" s="33">
+        <v>0.30099999999999999</v>
+      </c>
       <c r="M71" s="99">
         <v>66</v>
       </c>
@@ -21515,9 +22127,13 @@
       <c r="J72" s="38">
         <v>128</v>
       </c>
-      <c r="K72" s="38"/>
-      <c r="L72" s="33"/>
-      <c r="M72" s="99">
+      <c r="K72" s="38">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="L72" s="33">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="M72" s="124">
         <v>67</v>
       </c>
       <c r="Q72" s="106"/>
@@ -21563,9 +22179,13 @@
       <c r="J73" s="38">
         <v>128</v>
       </c>
-      <c r="K73" s="38"/>
-      <c r="L73" s="33"/>
-      <c r="M73" s="99">
+      <c r="K73" s="38">
+        <v>0.97</v>
+      </c>
+      <c r="L73" s="33">
+        <v>0.121</v>
+      </c>
+      <c r="M73" s="124">
         <v>68</v>
       </c>
       <c r="Q73" s="106"/>
@@ -21611,8 +22231,12 @@
       <c r="J74" s="38">
         <v>128</v>
       </c>
-      <c r="K74" s="38"/>
-      <c r="L74" s="33"/>
+      <c r="K74" s="38">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="L74" s="33">
+        <v>0.159</v>
+      </c>
       <c r="M74" s="99">
         <v>69</v>
       </c>
@@ -22190,7 +22814,7 @@
       </c>
       <c r="CL86" s="102"/>
       <c r="CN86" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="CX86" s="102"/>
       <c r="CY86" s="106"/>
@@ -22630,7 +23254,7 @@
       <c r="CB112" s="106"/>
       <c r="CL112" s="102"/>
       <c r="CN112" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="CX112" s="102"/>
       <c r="CY112" s="106"/>
@@ -23054,7 +23678,7 @@
       <c r="CB137" s="106"/>
       <c r="CL137" s="102"/>
       <c r="CN137" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="CX137" s="102"/>
       <c r="CY137" s="106"/>
@@ -23494,7 +24118,7 @@
       <c r="CB163" s="106"/>
       <c r="CL163" s="102"/>
       <c r="CN163" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="CX163" s="102"/>
       <c r="CY163" s="106"/>
@@ -23915,7 +24539,7 @@
       </c>
       <c r="CL188" s="102"/>
       <c r="CN188" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="CX188" s="102"/>
       <c r="CY188" s="106"/>
@@ -24355,7 +24979,7 @@
       </c>
       <c r="CL214" s="102"/>
       <c r="CN214" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="CX214" s="102"/>
       <c r="CY214" s="106"/>
@@ -24798,7 +25422,7 @@
       <c r="CB240" s="106"/>
       <c r="CL240" s="102"/>
       <c r="CN240" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="CX240" s="102"/>
       <c r="CY240" s="106"/>
@@ -25206,7 +25830,7 @@
       </c>
       <c r="CL264" s="102"/>
       <c r="CN264" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="CX264" s="102"/>
       <c r="CY264" s="106"/>
@@ -25726,22 +26350,22 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="136" t="s">
+      <c r="A4" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="137"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="139" t="s">
+      <c r="B4" s="138"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="137"/>
-      <c r="F4" s="138"/>
-      <c r="G4" s="137" t="s">
+      <c r="E4" s="138"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="138" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="137"/>
-      <c r="I4" s="137"/>
-      <c r="J4" s="140"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="141"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">

</xml_diff>

<commit_message>
finished analysis for learning rate of 0.1 and 0.01
</commit_message>
<xml_diff>
--- a/Python/4. NN/nn_analysis.xlsx
+++ b/Python/4. NN/nn_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\4. NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36E5B32-99F9-4CB7-B41C-F145FD6E61A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A29C33E-4A4C-4A8C-847F-E910507C9CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E68F98E9-ABC9-414C-A465-08CF722D05B6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="133">
   <si>
     <t xml:space="preserve">Model: </t>
   </si>
@@ -410,6 +410,36 @@
   </si>
   <si>
     <t>#70</t>
+  </si>
+  <si>
+    <t>#71</t>
+  </si>
+  <si>
+    <t>#72</t>
+  </si>
+  <si>
+    <t>#73</t>
+  </si>
+  <si>
+    <t>#74</t>
+  </si>
+  <si>
+    <t>#75</t>
+  </si>
+  <si>
+    <t>#76</t>
+  </si>
+  <si>
+    <t>#77</t>
+  </si>
+  <si>
+    <t>#78</t>
+  </si>
+  <si>
+    <t>#79</t>
+  </si>
+  <si>
+    <t>#80</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1528,6 +1558,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1579,7 +1612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8536,6 +8569,616 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="Picture 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9C717B4-0A69-21CF-0403-8CAAD8F8BF5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId74">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="6934200"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="Picture 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1AE427A-067F-0E93-2FBF-E68222E0F87A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId75">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="11715750"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Picture 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A75D543E-AA2A-E4FC-4AAE-388E9B0E4659}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId76">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="16506825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Picture 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF8D1475-8DD1-90F1-7D98-05597A3E2CB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId77">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="21459825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{598794EA-A670-EC7D-DDC7-86D08D23C146}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId78">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="26222325"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Picture 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B16FCC20-F424-6352-F9C9-A22FB0164004}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId79">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="31175325"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>211</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Picture 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{030D8534-4DD2-0A4F-14FD-6BF9734D59E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId80">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="36128325"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>237</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="77" name="Picture 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{918E1889-200B-C4C3-EB8C-65405924393A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId81">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="41081325"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="78" name="Picture 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{917E8C7C-5190-9AEF-BEAA-8DB74D759EB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId82">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="45843825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="79" name="Picture 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8531106C-931D-0FBF-D593-5145ABC8DC47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId83">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="65389125" y="50415825"/>
+          <a:ext cx="5400675" cy="4333875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8945,22 +9588,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="127"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="126" t="s">
+      <c r="B5" s="128"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="127" t="s">
+      <c r="E5" s="128"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="129"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -10365,22 +11008,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="127"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="126" t="s">
+      <c r="B5" s="128"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="127" t="s">
+      <c r="E5" s="128"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="129"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -11785,22 +12428,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="127"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="126" t="s">
+      <c r="B5" s="128"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="127" t="s">
+      <c r="E5" s="128"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="129"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -13205,22 +13848,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="127"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="126" t="s">
+      <c r="B5" s="128"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="127" t="s">
+      <c r="E5" s="128"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="129"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -14625,22 +15268,22 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="127"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="126" t="s">
+      <c r="B5" s="128"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="127" t="s">
+      <c r="E5" s="128"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="129"/>
       <c r="N5" t="s">
         <v>25</v>
       </c>
@@ -16025,22 +16668,22 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="127"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="126" t="s">
+      <c r="B5" s="128"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="127"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="127" t="s">
+      <c r="E5" s="128"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="129"/>
       <c r="K5" s="95"/>
       <c r="L5" s="108"/>
       <c r="M5" s="108"/>
@@ -18552,8 +19195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546EE643-96AE-406E-920D-B005CB201B4A}">
   <dimension ref="B3:DI291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K77" sqref="K77"/>
+    <sheetView tabSelected="1" topLeftCell="CA212" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P67" sqref="P67:P68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18571,25 +19214,25 @@
   <sheetData>
     <row r="3" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="127"/>
-      <c r="D4" s="128"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="129"/>
       <c r="E4" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="126" t="s">
+      <c r="F4" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="127"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="127" t="s">
+      <c r="G4" s="128"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="129"/>
       <c r="M4" s="95"/>
       <c r="N4" s="123"/>
       <c r="O4" s="122" t="s">
@@ -19680,102 +20323,102 @@
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="Q31" s="129" t="s">
+      <c r="Q31" s="130" t="s">
         <v>90</v>
       </c>
-      <c r="R31" s="130"/>
-      <c r="S31" s="130"/>
-      <c r="T31" s="130"/>
-      <c r="U31" s="130"/>
-      <c r="V31" s="130"/>
-      <c r="W31" s="130"/>
-      <c r="X31" s="130"/>
-      <c r="Y31" s="130"/>
-      <c r="Z31" s="130"/>
-      <c r="AA31" s="130"/>
-      <c r="AB31" s="130"/>
-      <c r="AC31" s="130"/>
-      <c r="AD31" s="130"/>
-      <c r="AE31" s="130"/>
-      <c r="AF31" s="130"/>
-      <c r="AG31" s="130"/>
-      <c r="AH31" s="130"/>
-      <c r="AI31" s="130"/>
-      <c r="AJ31" s="130"/>
-      <c r="AK31" s="130"/>
-      <c r="AL31" s="130"/>
-      <c r="AM31" s="130"/>
-      <c r="AN31" s="130"/>
-      <c r="AO31" s="130"/>
-      <c r="AP31" s="130"/>
-      <c r="AQ31" s="130"/>
-      <c r="AR31" s="130"/>
-      <c r="AS31" s="130"/>
-      <c r="AT31" s="130"/>
-      <c r="AU31" s="130"/>
-      <c r="AV31" s="130"/>
-      <c r="AW31" s="130"/>
-      <c r="AX31" s="130"/>
-      <c r="AY31" s="130"/>
-      <c r="AZ31" s="130"/>
-      <c r="BA31" s="130"/>
-      <c r="BB31" s="130"/>
-      <c r="BC31" s="130"/>
-      <c r="BD31" s="130"/>
-      <c r="BE31" s="130"/>
-      <c r="BF31" s="130"/>
-      <c r="BG31" s="130"/>
-      <c r="BH31" s="130"/>
-      <c r="BI31" s="130"/>
-      <c r="BJ31" s="131"/>
-      <c r="BP31" s="129" t="s">
+      <c r="R31" s="131"/>
+      <c r="S31" s="131"/>
+      <c r="T31" s="131"/>
+      <c r="U31" s="131"/>
+      <c r="V31" s="131"/>
+      <c r="W31" s="131"/>
+      <c r="X31" s="131"/>
+      <c r="Y31" s="131"/>
+      <c r="Z31" s="131"/>
+      <c r="AA31" s="131"/>
+      <c r="AB31" s="131"/>
+      <c r="AC31" s="131"/>
+      <c r="AD31" s="131"/>
+      <c r="AE31" s="131"/>
+      <c r="AF31" s="131"/>
+      <c r="AG31" s="131"/>
+      <c r="AH31" s="131"/>
+      <c r="AI31" s="131"/>
+      <c r="AJ31" s="131"/>
+      <c r="AK31" s="131"/>
+      <c r="AL31" s="131"/>
+      <c r="AM31" s="131"/>
+      <c r="AN31" s="131"/>
+      <c r="AO31" s="131"/>
+      <c r="AP31" s="131"/>
+      <c r="AQ31" s="131"/>
+      <c r="AR31" s="131"/>
+      <c r="AS31" s="131"/>
+      <c r="AT31" s="131"/>
+      <c r="AU31" s="131"/>
+      <c r="AV31" s="131"/>
+      <c r="AW31" s="131"/>
+      <c r="AX31" s="131"/>
+      <c r="AY31" s="131"/>
+      <c r="AZ31" s="131"/>
+      <c r="BA31" s="131"/>
+      <c r="BB31" s="131"/>
+      <c r="BC31" s="131"/>
+      <c r="BD31" s="131"/>
+      <c r="BE31" s="131"/>
+      <c r="BF31" s="131"/>
+      <c r="BG31" s="131"/>
+      <c r="BH31" s="131"/>
+      <c r="BI31" s="131"/>
+      <c r="BJ31" s="132"/>
+      <c r="BP31" s="130" t="s">
         <v>92</v>
       </c>
-      <c r="BQ31" s="130"/>
-      <c r="BR31" s="130"/>
-      <c r="BS31" s="130"/>
-      <c r="BT31" s="130"/>
-      <c r="BU31" s="130"/>
-      <c r="BV31" s="130"/>
-      <c r="BW31" s="130"/>
-      <c r="BX31" s="130"/>
-      <c r="BY31" s="130"/>
-      <c r="BZ31" s="130"/>
-      <c r="CA31" s="130"/>
-      <c r="CB31" s="130"/>
-      <c r="CC31" s="130"/>
-      <c r="CD31" s="130"/>
-      <c r="CE31" s="130"/>
-      <c r="CF31" s="130"/>
-      <c r="CG31" s="130"/>
-      <c r="CH31" s="130"/>
-      <c r="CI31" s="130"/>
-      <c r="CJ31" s="130"/>
-      <c r="CK31" s="130"/>
-      <c r="CL31" s="130"/>
-      <c r="CM31" s="130"/>
-      <c r="CN31" s="130"/>
-      <c r="CO31" s="130"/>
-      <c r="CP31" s="130"/>
-      <c r="CQ31" s="130"/>
-      <c r="CR31" s="130"/>
-      <c r="CS31" s="130"/>
-      <c r="CT31" s="130"/>
-      <c r="CU31" s="130"/>
-      <c r="CV31" s="130"/>
-      <c r="CW31" s="130"/>
-      <c r="CX31" s="130"/>
-      <c r="CY31" s="130"/>
-      <c r="CZ31" s="130"/>
-      <c r="DA31" s="130"/>
-      <c r="DB31" s="130"/>
-      <c r="DC31" s="130"/>
-      <c r="DD31" s="130"/>
-      <c r="DE31" s="130"/>
-      <c r="DF31" s="130"/>
-      <c r="DG31" s="130"/>
-      <c r="DH31" s="130"/>
-      <c r="DI31" s="131"/>
+      <c r="BQ31" s="131"/>
+      <c r="BR31" s="131"/>
+      <c r="BS31" s="131"/>
+      <c r="BT31" s="131"/>
+      <c r="BU31" s="131"/>
+      <c r="BV31" s="131"/>
+      <c r="BW31" s="131"/>
+      <c r="BX31" s="131"/>
+      <c r="BY31" s="131"/>
+      <c r="BZ31" s="131"/>
+      <c r="CA31" s="131"/>
+      <c r="CB31" s="131"/>
+      <c r="CC31" s="131"/>
+      <c r="CD31" s="131"/>
+      <c r="CE31" s="131"/>
+      <c r="CF31" s="131"/>
+      <c r="CG31" s="131"/>
+      <c r="CH31" s="131"/>
+      <c r="CI31" s="131"/>
+      <c r="CJ31" s="131"/>
+      <c r="CK31" s="131"/>
+      <c r="CL31" s="131"/>
+      <c r="CM31" s="131"/>
+      <c r="CN31" s="131"/>
+      <c r="CO31" s="131"/>
+      <c r="CP31" s="131"/>
+      <c r="CQ31" s="131"/>
+      <c r="CR31" s="131"/>
+      <c r="CS31" s="131"/>
+      <c r="CT31" s="131"/>
+      <c r="CU31" s="131"/>
+      <c r="CV31" s="131"/>
+      <c r="CW31" s="131"/>
+      <c r="CX31" s="131"/>
+      <c r="CY31" s="131"/>
+      <c r="CZ31" s="131"/>
+      <c r="DA31" s="131"/>
+      <c r="DB31" s="131"/>
+      <c r="DC31" s="131"/>
+      <c r="DD31" s="131"/>
+      <c r="DE31" s="131"/>
+      <c r="DF31" s="131"/>
+      <c r="DG31" s="131"/>
+      <c r="DH31" s="131"/>
+      <c r="DI31" s="132"/>
     </row>
     <row r="32" spans="2:113" x14ac:dyDescent="0.25">
       <c r="B32" s="31">
@@ -19816,98 +20459,98 @@
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="Q32" s="132"/>
-      <c r="R32" s="133"/>
-      <c r="S32" s="133"/>
-      <c r="T32" s="133"/>
-      <c r="U32" s="133"/>
-      <c r="V32" s="133"/>
-      <c r="W32" s="133"/>
-      <c r="X32" s="133"/>
-      <c r="Y32" s="133"/>
-      <c r="Z32" s="133"/>
-      <c r="AA32" s="133"/>
-      <c r="AB32" s="133"/>
-      <c r="AC32" s="133"/>
-      <c r="AD32" s="133"/>
-      <c r="AE32" s="133"/>
-      <c r="AF32" s="133"/>
-      <c r="AG32" s="133"/>
-      <c r="AH32" s="133"/>
-      <c r="AI32" s="133"/>
-      <c r="AJ32" s="133"/>
-      <c r="AK32" s="133"/>
-      <c r="AL32" s="133"/>
-      <c r="AM32" s="133"/>
-      <c r="AN32" s="133"/>
-      <c r="AO32" s="133"/>
-      <c r="AP32" s="133"/>
-      <c r="AQ32" s="133"/>
-      <c r="AR32" s="133"/>
-      <c r="AS32" s="133"/>
-      <c r="AT32" s="133"/>
-      <c r="AU32" s="133"/>
-      <c r="AV32" s="133"/>
-      <c r="AW32" s="133"/>
-      <c r="AX32" s="133"/>
-      <c r="AY32" s="133"/>
-      <c r="AZ32" s="133"/>
-      <c r="BA32" s="133"/>
-      <c r="BB32" s="133"/>
-      <c r="BC32" s="133"/>
-      <c r="BD32" s="133"/>
-      <c r="BE32" s="133"/>
-      <c r="BF32" s="133"/>
-      <c r="BG32" s="133"/>
-      <c r="BH32" s="133"/>
-      <c r="BI32" s="133"/>
-      <c r="BJ32" s="134"/>
-      <c r="BP32" s="132"/>
-      <c r="BQ32" s="133"/>
-      <c r="BR32" s="133"/>
-      <c r="BS32" s="133"/>
-      <c r="BT32" s="133"/>
-      <c r="BU32" s="133"/>
-      <c r="BV32" s="133"/>
-      <c r="BW32" s="133"/>
-      <c r="BX32" s="133"/>
-      <c r="BY32" s="133"/>
-      <c r="BZ32" s="133"/>
-      <c r="CA32" s="133"/>
-      <c r="CB32" s="133"/>
-      <c r="CC32" s="133"/>
-      <c r="CD32" s="133"/>
-      <c r="CE32" s="133"/>
-      <c r="CF32" s="133"/>
-      <c r="CG32" s="133"/>
-      <c r="CH32" s="133"/>
-      <c r="CI32" s="133"/>
-      <c r="CJ32" s="133"/>
-      <c r="CK32" s="133"/>
-      <c r="CL32" s="133"/>
-      <c r="CM32" s="133"/>
-      <c r="CN32" s="133"/>
-      <c r="CO32" s="133"/>
-      <c r="CP32" s="133"/>
-      <c r="CQ32" s="133"/>
-      <c r="CR32" s="133"/>
-      <c r="CS32" s="133"/>
-      <c r="CT32" s="133"/>
-      <c r="CU32" s="133"/>
-      <c r="CV32" s="133"/>
-      <c r="CW32" s="133"/>
-      <c r="CX32" s="133"/>
-      <c r="CY32" s="133"/>
-      <c r="CZ32" s="133"/>
-      <c r="DA32" s="133"/>
-      <c r="DB32" s="133"/>
-      <c r="DC32" s="133"/>
-      <c r="DD32" s="133"/>
-      <c r="DE32" s="133"/>
-      <c r="DF32" s="133"/>
-      <c r="DG32" s="133"/>
-      <c r="DH32" s="133"/>
-      <c r="DI32" s="134"/>
+      <c r="Q32" s="133"/>
+      <c r="R32" s="134"/>
+      <c r="S32" s="134"/>
+      <c r="T32" s="134"/>
+      <c r="U32" s="134"/>
+      <c r="V32" s="134"/>
+      <c r="W32" s="134"/>
+      <c r="X32" s="134"/>
+      <c r="Y32" s="134"/>
+      <c r="Z32" s="134"/>
+      <c r="AA32" s="134"/>
+      <c r="AB32" s="134"/>
+      <c r="AC32" s="134"/>
+      <c r="AD32" s="134"/>
+      <c r="AE32" s="134"/>
+      <c r="AF32" s="134"/>
+      <c r="AG32" s="134"/>
+      <c r="AH32" s="134"/>
+      <c r="AI32" s="134"/>
+      <c r="AJ32" s="134"/>
+      <c r="AK32" s="134"/>
+      <c r="AL32" s="134"/>
+      <c r="AM32" s="134"/>
+      <c r="AN32" s="134"/>
+      <c r="AO32" s="134"/>
+      <c r="AP32" s="134"/>
+      <c r="AQ32" s="134"/>
+      <c r="AR32" s="134"/>
+      <c r="AS32" s="134"/>
+      <c r="AT32" s="134"/>
+      <c r="AU32" s="134"/>
+      <c r="AV32" s="134"/>
+      <c r="AW32" s="134"/>
+      <c r="AX32" s="134"/>
+      <c r="AY32" s="134"/>
+      <c r="AZ32" s="134"/>
+      <c r="BA32" s="134"/>
+      <c r="BB32" s="134"/>
+      <c r="BC32" s="134"/>
+      <c r="BD32" s="134"/>
+      <c r="BE32" s="134"/>
+      <c r="BF32" s="134"/>
+      <c r="BG32" s="134"/>
+      <c r="BH32" s="134"/>
+      <c r="BI32" s="134"/>
+      <c r="BJ32" s="135"/>
+      <c r="BP32" s="133"/>
+      <c r="BQ32" s="134"/>
+      <c r="BR32" s="134"/>
+      <c r="BS32" s="134"/>
+      <c r="BT32" s="134"/>
+      <c r="BU32" s="134"/>
+      <c r="BV32" s="134"/>
+      <c r="BW32" s="134"/>
+      <c r="BX32" s="134"/>
+      <c r="BY32" s="134"/>
+      <c r="BZ32" s="134"/>
+      <c r="CA32" s="134"/>
+      <c r="CB32" s="134"/>
+      <c r="CC32" s="134"/>
+      <c r="CD32" s="134"/>
+      <c r="CE32" s="134"/>
+      <c r="CF32" s="134"/>
+      <c r="CG32" s="134"/>
+      <c r="CH32" s="134"/>
+      <c r="CI32" s="134"/>
+      <c r="CJ32" s="134"/>
+      <c r="CK32" s="134"/>
+      <c r="CL32" s="134"/>
+      <c r="CM32" s="134"/>
+      <c r="CN32" s="134"/>
+      <c r="CO32" s="134"/>
+      <c r="CP32" s="134"/>
+      <c r="CQ32" s="134"/>
+      <c r="CR32" s="134"/>
+      <c r="CS32" s="134"/>
+      <c r="CT32" s="134"/>
+      <c r="CU32" s="134"/>
+      <c r="CV32" s="134"/>
+      <c r="CW32" s="134"/>
+      <c r="CX32" s="134"/>
+      <c r="CY32" s="134"/>
+      <c r="CZ32" s="134"/>
+      <c r="DA32" s="134"/>
+      <c r="DB32" s="134"/>
+      <c r="DC32" s="134"/>
+      <c r="DD32" s="134"/>
+      <c r="DE32" s="134"/>
+      <c r="DF32" s="134"/>
+      <c r="DG32" s="134"/>
+      <c r="DH32" s="134"/>
+      <c r="DI32" s="135"/>
     </row>
     <row r="33" spans="2:113" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="31">
@@ -19948,98 +20591,98 @@
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="Q33" s="135"/>
-      <c r="R33" s="136"/>
-      <c r="S33" s="136"/>
-      <c r="T33" s="136"/>
-      <c r="U33" s="136"/>
-      <c r="V33" s="136"/>
-      <c r="W33" s="136"/>
-      <c r="X33" s="136"/>
-      <c r="Y33" s="136"/>
-      <c r="Z33" s="136"/>
-      <c r="AA33" s="136"/>
-      <c r="AB33" s="136"/>
-      <c r="AC33" s="136"/>
-      <c r="AD33" s="136"/>
-      <c r="AE33" s="136"/>
-      <c r="AF33" s="136"/>
-      <c r="AG33" s="136"/>
-      <c r="AH33" s="136"/>
-      <c r="AI33" s="136"/>
-      <c r="AJ33" s="136"/>
-      <c r="AK33" s="136"/>
-      <c r="AL33" s="136"/>
-      <c r="AM33" s="136"/>
-      <c r="AN33" s="136"/>
-      <c r="AO33" s="136"/>
-      <c r="AP33" s="136"/>
-      <c r="AQ33" s="136"/>
-      <c r="AR33" s="136"/>
-      <c r="AS33" s="136"/>
-      <c r="AT33" s="136"/>
-      <c r="AU33" s="136"/>
-      <c r="AV33" s="136"/>
-      <c r="AW33" s="136"/>
-      <c r="AX33" s="136"/>
-      <c r="AY33" s="136"/>
-      <c r="AZ33" s="136"/>
-      <c r="BA33" s="136"/>
-      <c r="BB33" s="136"/>
-      <c r="BC33" s="136"/>
-      <c r="BD33" s="136"/>
-      <c r="BE33" s="136"/>
-      <c r="BF33" s="136"/>
-      <c r="BG33" s="136"/>
-      <c r="BH33" s="136"/>
-      <c r="BI33" s="136"/>
-      <c r="BJ33" s="137"/>
-      <c r="BP33" s="135"/>
-      <c r="BQ33" s="136"/>
-      <c r="BR33" s="136"/>
-      <c r="BS33" s="136"/>
-      <c r="BT33" s="136"/>
-      <c r="BU33" s="136"/>
-      <c r="BV33" s="136"/>
-      <c r="BW33" s="136"/>
-      <c r="BX33" s="136"/>
-      <c r="BY33" s="136"/>
-      <c r="BZ33" s="136"/>
-      <c r="CA33" s="136"/>
-      <c r="CB33" s="136"/>
-      <c r="CC33" s="136"/>
-      <c r="CD33" s="136"/>
-      <c r="CE33" s="136"/>
-      <c r="CF33" s="136"/>
-      <c r="CG33" s="136"/>
-      <c r="CH33" s="136"/>
-      <c r="CI33" s="136"/>
-      <c r="CJ33" s="136"/>
-      <c r="CK33" s="136"/>
-      <c r="CL33" s="136"/>
-      <c r="CM33" s="136"/>
-      <c r="CN33" s="136"/>
-      <c r="CO33" s="136"/>
-      <c r="CP33" s="136"/>
-      <c r="CQ33" s="136"/>
-      <c r="CR33" s="136"/>
-      <c r="CS33" s="136"/>
-      <c r="CT33" s="136"/>
-      <c r="CU33" s="136"/>
-      <c r="CV33" s="136"/>
-      <c r="CW33" s="136"/>
-      <c r="CX33" s="136"/>
-      <c r="CY33" s="136"/>
-      <c r="CZ33" s="136"/>
-      <c r="DA33" s="136"/>
-      <c r="DB33" s="136"/>
-      <c r="DC33" s="136"/>
-      <c r="DD33" s="136"/>
-      <c r="DE33" s="136"/>
-      <c r="DF33" s="136"/>
-      <c r="DG33" s="136"/>
-      <c r="DH33" s="136"/>
-      <c r="DI33" s="137"/>
+      <c r="Q33" s="136"/>
+      <c r="R33" s="137"/>
+      <c r="S33" s="137"/>
+      <c r="T33" s="137"/>
+      <c r="U33" s="137"/>
+      <c r="V33" s="137"/>
+      <c r="W33" s="137"/>
+      <c r="X33" s="137"/>
+      <c r="Y33" s="137"/>
+      <c r="Z33" s="137"/>
+      <c r="AA33" s="137"/>
+      <c r="AB33" s="137"/>
+      <c r="AC33" s="137"/>
+      <c r="AD33" s="137"/>
+      <c r="AE33" s="137"/>
+      <c r="AF33" s="137"/>
+      <c r="AG33" s="137"/>
+      <c r="AH33" s="137"/>
+      <c r="AI33" s="137"/>
+      <c r="AJ33" s="137"/>
+      <c r="AK33" s="137"/>
+      <c r="AL33" s="137"/>
+      <c r="AM33" s="137"/>
+      <c r="AN33" s="137"/>
+      <c r="AO33" s="137"/>
+      <c r="AP33" s="137"/>
+      <c r="AQ33" s="137"/>
+      <c r="AR33" s="137"/>
+      <c r="AS33" s="137"/>
+      <c r="AT33" s="137"/>
+      <c r="AU33" s="137"/>
+      <c r="AV33" s="137"/>
+      <c r="AW33" s="137"/>
+      <c r="AX33" s="137"/>
+      <c r="AY33" s="137"/>
+      <c r="AZ33" s="137"/>
+      <c r="BA33" s="137"/>
+      <c r="BB33" s="137"/>
+      <c r="BC33" s="137"/>
+      <c r="BD33" s="137"/>
+      <c r="BE33" s="137"/>
+      <c r="BF33" s="137"/>
+      <c r="BG33" s="137"/>
+      <c r="BH33" s="137"/>
+      <c r="BI33" s="137"/>
+      <c r="BJ33" s="138"/>
+      <c r="BP33" s="136"/>
+      <c r="BQ33" s="137"/>
+      <c r="BR33" s="137"/>
+      <c r="BS33" s="137"/>
+      <c r="BT33" s="137"/>
+      <c r="BU33" s="137"/>
+      <c r="BV33" s="137"/>
+      <c r="BW33" s="137"/>
+      <c r="BX33" s="137"/>
+      <c r="BY33" s="137"/>
+      <c r="BZ33" s="137"/>
+      <c r="CA33" s="137"/>
+      <c r="CB33" s="137"/>
+      <c r="CC33" s="137"/>
+      <c r="CD33" s="137"/>
+      <c r="CE33" s="137"/>
+      <c r="CF33" s="137"/>
+      <c r="CG33" s="137"/>
+      <c r="CH33" s="137"/>
+      <c r="CI33" s="137"/>
+      <c r="CJ33" s="137"/>
+      <c r="CK33" s="137"/>
+      <c r="CL33" s="137"/>
+      <c r="CM33" s="137"/>
+      <c r="CN33" s="137"/>
+      <c r="CO33" s="137"/>
+      <c r="CP33" s="137"/>
+      <c r="CQ33" s="137"/>
+      <c r="CR33" s="137"/>
+      <c r="CS33" s="137"/>
+      <c r="CT33" s="137"/>
+      <c r="CU33" s="137"/>
+      <c r="CV33" s="137"/>
+      <c r="CW33" s="137"/>
+      <c r="CX33" s="137"/>
+      <c r="CY33" s="137"/>
+      <c r="CZ33" s="137"/>
+      <c r="DA33" s="137"/>
+      <c r="DB33" s="137"/>
+      <c r="DC33" s="137"/>
+      <c r="DD33" s="137"/>
+      <c r="DE33" s="137"/>
+      <c r="DF33" s="137"/>
+      <c r="DG33" s="137"/>
+      <c r="DH33" s="137"/>
+      <c r="DI33" s="138"/>
     </row>
     <row r="34" spans="2:113" x14ac:dyDescent="0.25">
       <c r="B34" s="31">
@@ -20301,7 +20944,7 @@
       <c r="CX36" s="102"/>
       <c r="CY36" s="106"/>
       <c r="CZ36" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="DI36" s="102"/>
     </row>
@@ -21639,7 +22282,7 @@
       <c r="CX61" s="102"/>
       <c r="CY61" s="106"/>
       <c r="CZ61" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="DI61" s="102"/>
     </row>
@@ -22320,40 +22963,40 @@
       <c r="DI74" s="102"/>
     </row>
     <row r="75" spans="2:113" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="16">
+      <c r="B75" s="61">
         <v>3</v>
       </c>
-      <c r="C75" s="41" t="s">
+      <c r="C75" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D75" s="19" t="s">
+      <c r="D75" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="E75" s="3">
+      <c r="E75" s="80">
         <v>0.01</v>
       </c>
-      <c r="F75" s="45" t="s">
+      <c r="F75" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="G75" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="H75" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I75" s="17">
+      <c r="G75" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="H75" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="I75" s="144">
         <v>450</v>
       </c>
-      <c r="J75" s="41">
+      <c r="J75" s="65">
         <v>128</v>
       </c>
-      <c r="K75" s="41">
+      <c r="K75" s="65">
         <v>0.98</v>
       </c>
-      <c r="L75" s="19">
+      <c r="L75" s="63">
         <v>0.109</v>
       </c>
-      <c r="M75" s="143">
+      <c r="M75" s="126">
         <v>70</v>
       </c>
       <c r="Q75" s="106"/>
@@ -22399,8 +23042,12 @@
       <c r="J76" s="114">
         <v>256</v>
       </c>
-      <c r="K76" s="114"/>
-      <c r="L76" s="115"/>
+      <c r="K76" s="114">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="L76" s="115">
+        <v>1.575</v>
+      </c>
       <c r="M76" s="119">
         <v>71</v>
       </c>
@@ -22447,8 +23094,12 @@
       <c r="J77" s="38">
         <v>256</v>
       </c>
-      <c r="K77" s="38"/>
-      <c r="L77" s="33"/>
+      <c r="K77" s="38">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="L77" s="33">
+        <v>0.89600000000000002</v>
+      </c>
       <c r="M77" s="99">
         <v>72</v>
       </c>
@@ -22495,8 +23146,12 @@
       <c r="J78" s="38">
         <v>256</v>
       </c>
-      <c r="K78" s="38"/>
-      <c r="L78" s="33"/>
+      <c r="K78" s="38">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="L78" s="33">
+        <v>0.69199999999999995</v>
+      </c>
       <c r="M78" s="99">
         <v>73</v>
       </c>
@@ -22543,8 +23198,12 @@
       <c r="J79" s="38">
         <v>256</v>
       </c>
-      <c r="K79" s="38"/>
-      <c r="L79" s="33"/>
+      <c r="K79" s="38">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="L79" s="33">
+        <v>0.40799999999999997</v>
+      </c>
       <c r="M79" s="99">
         <v>74</v>
       </c>
@@ -22591,8 +23250,12 @@
       <c r="J80" s="38">
         <v>256</v>
       </c>
-      <c r="K80" s="38"/>
-      <c r="L80" s="33"/>
+      <c r="K80" s="38">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="L80" s="33">
+        <v>0.58899999999999997</v>
+      </c>
       <c r="M80" s="99">
         <v>75</v>
       </c>
@@ -22639,8 +23302,12 @@
       <c r="J81" s="38">
         <v>256</v>
       </c>
-      <c r="K81" s="38"/>
-      <c r="L81" s="33"/>
+      <c r="K81" s="38">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="L81" s="33">
+        <v>0.19900000000000001</v>
+      </c>
       <c r="M81" s="99">
         <v>76</v>
       </c>
@@ -22687,8 +23354,12 @@
       <c r="J82" s="38">
         <v>256</v>
       </c>
-      <c r="K82" s="38"/>
-      <c r="L82" s="33"/>
+      <c r="K82" s="38">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="L82" s="33">
+        <v>0.38900000000000001</v>
+      </c>
       <c r="M82" s="99">
         <v>77</v>
       </c>
@@ -22735,9 +23406,13 @@
       <c r="J83" s="38">
         <v>256</v>
       </c>
-      <c r="K83" s="38"/>
-      <c r="L83" s="33"/>
-      <c r="M83" s="99">
+      <c r="K83" s="38">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="L83" s="33">
+        <v>0.189</v>
+      </c>
+      <c r="M83" s="124">
         <v>78</v>
       </c>
       <c r="Q83" s="106"/>
@@ -22783,8 +23458,12 @@
       <c r="J84" s="38">
         <v>256</v>
       </c>
-      <c r="K84" s="38"/>
-      <c r="L84" s="33"/>
+      <c r="K84" s="38">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="L84" s="33">
+        <v>0.33700000000000002</v>
+      </c>
       <c r="M84" s="99">
         <v>79</v>
       </c>
@@ -22831,8 +23510,12 @@
       <c r="J85" s="42">
         <v>256</v>
       </c>
-      <c r="K85" s="42"/>
-      <c r="L85" s="4"/>
+      <c r="K85" s="42">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="L85" s="4">
+        <v>0.36799999999999999</v>
+      </c>
       <c r="M85" s="97">
         <v>80</v>
       </c>
@@ -22887,7 +23570,7 @@
       <c r="CX86" s="102"/>
       <c r="CY86" s="106"/>
       <c r="CZ86" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="DI86" s="102"/>
     </row>
@@ -23327,7 +24010,7 @@
       <c r="CX112" s="102"/>
       <c r="CY112" s="106"/>
       <c r="CZ112" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="DI112" s="102"/>
     </row>
@@ -23751,7 +24434,7 @@
       <c r="CX137" s="102"/>
       <c r="CY137" s="106"/>
       <c r="CZ137" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="DI137" s="102"/>
     </row>
@@ -24191,7 +24874,7 @@
       <c r="CX163" s="102"/>
       <c r="CY163" s="106"/>
       <c r="CZ163" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="DI163" s="102"/>
     </row>
@@ -24631,7 +25314,7 @@
       <c r="CX189" s="102"/>
       <c r="CY189" s="106"/>
       <c r="CZ189" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="DI189" s="102"/>
     </row>
@@ -25071,7 +25754,7 @@
       <c r="CX215" s="102"/>
       <c r="CY215" s="106"/>
       <c r="CZ215" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="DI215" s="102"/>
     </row>
@@ -25495,7 +26178,7 @@
       <c r="CX240" s="102"/>
       <c r="CY240" s="106"/>
       <c r="CZ240" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
       <c r="DI240" s="102"/>
     </row>
@@ -25903,7 +26586,7 @@
       <c r="CX264" s="102"/>
       <c r="CY264" s="106"/>
       <c r="CZ264" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="DI264" s="102"/>
     </row>
@@ -26418,22 +27101,22 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="138" t="s">
+      <c r="A4" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="139"/>
-      <c r="C4" s="140"/>
-      <c r="D4" s="141" t="s">
+      <c r="B4" s="140"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="142" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="139"/>
-      <c r="F4" s="140"/>
-      <c r="G4" s="139" t="s">
+      <c r="E4" s="140"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="139"/>
-      <c r="I4" s="139"/>
-      <c r="J4" s="142"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="143"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">

</xml_diff>